<commit_message>
update call of parasites
</commit_message>
<xml_diff>
--- a/cards.xlsx
+++ b/cards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\_projects\_OFF\theParasitized\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7884BCF3-D994-4BB6-86AD-05F8D2E584AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F524905F-D286-46B8-AAF4-AE1766FC83B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="140">
   <si>
     <t>NO.01</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -403,6 +403,114 @@
   </si>
   <si>
     <t>技能</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>造成6伤害</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获得5格挡</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>进化你的手牌3次</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>能力</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>羽化</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>抽1弃1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>选择</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>将手牌抽满</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>消耗1手牌获得1E, 若为诅咒牌, 则再获得1E</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>造成3次3伤害</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>连击</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>若斩杀的是精英怪, 升级你的全部诅咒</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>发现1诅咒</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>造成2伤害, 恢复2生命, 每有1诅咒, 重复1次</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>回合开始时, 添加1诅咒, 你的手牌没有上限</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>消耗3张牌, 使其变为随机诅咒</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>消耗你的全部手牌,每张手牌对所有敌人造成伤害</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>回合结束时, 将一张生长加入你的抽牌堆, 生长: 0费抽1, 升级1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>打7抽1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获得4格挡, 恢复2生命</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>战斗结束时, 获得1张诅咒牌, 恢复6生命</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>可以打出诅咒牌, 打出诅咒牌的时候, 抽2张牌</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>消耗1张手牌, 获得9点格挡</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>抽到时,随机升级一张手牌</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>抽2张牌, 打出4张后结束回合</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>对所有敌人造成伤害</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>亵渎</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -862,22 +970,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="D2:Z81"/>
+  <dimension ref="D2:AB81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="W16" sqref="W16"/>
+    <sheetView tabSelected="1" topLeftCell="B11" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27:U27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="17" max="17" width="8.77734375" style="1" customWidth="1"/>
-    <col min="18" max="18" width="14.109375" style="1" customWidth="1"/>
-    <col min="19" max="19" width="8.77734375" customWidth="1"/>
-    <col min="20" max="24" width="8.77734375" style="1" customWidth="1"/>
-    <col min="25" max="25" width="8.88671875" style="1"/>
+    <col min="19" max="19" width="8.77734375" style="1" customWidth="1"/>
+    <col min="20" max="20" width="14.109375" style="1" customWidth="1"/>
+    <col min="21" max="21" width="8.77734375" customWidth="1"/>
+    <col min="22" max="26" width="8.77734375" style="1" customWidth="1"/>
+    <col min="27" max="27" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:26" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="4:28" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
         <v>77</v>
       </c>
@@ -896,22 +1004,28 @@
       <c r="Q2" s="3"/>
       <c r="R2" s="3"/>
       <c r="S2" s="3"/>
-      <c r="T2" s="7"/>
-      <c r="U2" s="7"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
       <c r="V2" s="7"/>
       <c r="W2" s="7"/>
       <c r="X2" s="7"/>
       <c r="Y2" s="7"/>
-      <c r="Z2" s="4"/>
-    </row>
-    <row r="6" spans="4:26" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z2" s="7"/>
+      <c r="AA2" s="7"/>
+      <c r="AB2" s="4"/>
+    </row>
+    <row r="6" spans="4:28" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E6" s="8" t="s">
         <v>75</v>
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
+      <c r="H6" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>81</v>
+      </c>
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
       <c r="L6" s="8"/>
@@ -922,26 +1036,22 @@
       <c r="Q6" s="8"/>
       <c r="R6" s="8"/>
       <c r="S6" s="8"/>
-      <c r="T6" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="U6" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="V6" s="1" t="s">
+      <c r="T6" s="8"/>
+      <c r="U6" s="8"/>
+      <c r="X6" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="W6" s="1" t="s">
+      <c r="Y6" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="X6" s="1" t="s">
+      <c r="Z6" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="Y6" s="1" t="s">
+      <c r="AA6" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="4:26" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="4:28" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
         <v>0</v>
       </c>
@@ -950,9 +1060,15 @@
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
+      <c r="H7" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I7" s="1">
+        <v>1</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>113</v>
+      </c>
       <c r="K7" s="8"/>
       <c r="L7" s="8"/>
       <c r="M7" s="8"/>
@@ -962,14 +1078,10 @@
       <c r="Q7" s="8"/>
       <c r="R7" s="8"/>
       <c r="S7" s="8"/>
-      <c r="T7" s="1">
-        <v>1</v>
-      </c>
-      <c r="U7" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="8" spans="4:26" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T7" s="8"/>
+      <c r="U7" s="8"/>
+    </row>
+    <row r="8" spans="4:28" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
         <v>1</v>
       </c>
@@ -978,9 +1090,15 @@
       </c>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
+      <c r="H8" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="I8" s="1">
+        <v>1</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>114</v>
+      </c>
       <c r="K8" s="8"/>
       <c r="L8" s="8"/>
       <c r="M8" s="8"/>
@@ -990,23 +1108,27 @@
       <c r="Q8" s="8"/>
       <c r="R8" s="8"/>
       <c r="S8" s="8"/>
-      <c r="T8" s="1">
-        <v>1</v>
-      </c>
-      <c r="U8" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="9" spans="4:26" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T8" s="8"/>
+      <c r="U8" s="8"/>
+    </row>
+    <row r="9" spans="4:28" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="8"/>
+      <c r="E9" s="8" t="s">
+        <v>117</v>
+      </c>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
+      <c r="H9" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="I9" s="1">
+        <v>2</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>115</v>
+      </c>
       <c r="K9" s="8"/>
       <c r="L9" s="8"/>
       <c r="M9" s="8"/>
@@ -1016,17 +1138,27 @@
       <c r="Q9" s="8"/>
       <c r="R9" s="8"/>
       <c r="S9" s="8"/>
-    </row>
-    <row r="10" spans="4:26" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T9" s="8"/>
+      <c r="U9" s="8"/>
+    </row>
+    <row r="10" spans="4:28" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="8"/>
+      <c r="E10" s="8" t="s">
+        <v>119</v>
+      </c>
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
+      <c r="H10" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I10" s="1">
+        <v>1</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>118</v>
+      </c>
       <c r="K10" s="8"/>
       <c r="L10" s="8"/>
       <c r="M10" s="8"/>
@@ -1036,17 +1168,25 @@
       <c r="Q10" s="8"/>
       <c r="R10" s="8"/>
       <c r="S10" s="8"/>
-    </row>
-    <row r="11" spans="4:26" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T10" s="8"/>
+      <c r="U10" s="8"/>
+    </row>
+    <row r="11" spans="4:28" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
         <v>4</v>
       </c>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
+      <c r="H11" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="I11" s="1">
+        <v>2</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>120</v>
+      </c>
       <c r="K11" s="8"/>
       <c r="L11" s="8"/>
       <c r="M11" s="8"/>
@@ -1056,17 +1196,25 @@
       <c r="Q11" s="8"/>
       <c r="R11" s="8"/>
       <c r="S11" s="8"/>
-    </row>
-    <row r="12" spans="4:26" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T11" s="8"/>
+      <c r="U11" s="8"/>
+    </row>
+    <row r="12" spans="4:28" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
         <v>5</v>
       </c>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
+      <c r="H12" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="I12" s="1">
+        <v>1</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>121</v>
+      </c>
       <c r="K12" s="8"/>
       <c r="L12" s="8"/>
       <c r="M12" s="8"/>
@@ -1076,17 +1224,27 @@
       <c r="Q12" s="8"/>
       <c r="R12" s="8"/>
       <c r="S12" s="8"/>
-    </row>
-    <row r="13" spans="4:26" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T12" s="8"/>
+      <c r="U12" s="8"/>
+    </row>
+    <row r="13" spans="4:28" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="8"/>
+      <c r="E13" s="8" t="s">
+        <v>123</v>
+      </c>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
+      <c r="H13" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I13" s="1">
+        <v>1</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>122</v>
+      </c>
       <c r="K13" s="8"/>
       <c r="L13" s="8"/>
       <c r="M13" s="8"/>
@@ -1096,17 +1254,25 @@
       <c r="Q13" s="8"/>
       <c r="R13" s="8"/>
       <c r="S13" s="8"/>
-    </row>
-    <row r="14" spans="4:26" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T13" s="8"/>
+      <c r="U13" s="8"/>
+    </row>
+    <row r="14" spans="4:28" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
         <v>7</v>
       </c>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
+      <c r="H14" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I14" s="1">
+        <v>3</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>124</v>
+      </c>
       <c r="K14" s="8"/>
       <c r="L14" s="8"/>
       <c r="M14" s="8"/>
@@ -1116,17 +1282,25 @@
       <c r="Q14" s="8"/>
       <c r="R14" s="8"/>
       <c r="S14" s="8"/>
-    </row>
-    <row r="15" spans="4:26" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T14" s="8"/>
+      <c r="U14" s="8"/>
+    </row>
+    <row r="15" spans="4:28" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
         <v>8</v>
       </c>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
+      <c r="H15" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="I15" s="1">
+        <v>1</v>
+      </c>
+      <c r="J15" s="8" t="s">
+        <v>125</v>
+      </c>
       <c r="K15" s="8"/>
       <c r="L15" s="8"/>
       <c r="M15" s="8"/>
@@ -1136,17 +1310,25 @@
       <c r="Q15" s="8"/>
       <c r="R15" s="8"/>
       <c r="S15" s="8"/>
-    </row>
-    <row r="16" spans="4:26" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T15" s="8"/>
+      <c r="U15" s="8"/>
+    </row>
+    <row r="16" spans="4:28" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
         <v>9</v>
       </c>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
+      <c r="H16" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I16" s="1">
+        <v>2</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>126</v>
+      </c>
       <c r="K16" s="8"/>
       <c r="L16" s="8"/>
       <c r="M16" s="8"/>
@@ -1156,17 +1338,25 @@
       <c r="Q16" s="8"/>
       <c r="R16" s="8"/>
       <c r="S16" s="8"/>
-    </row>
-    <row r="17" spans="4:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T16" s="8"/>
+      <c r="U16" s="8"/>
+    </row>
+    <row r="17" spans="4:21" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
         <v>10</v>
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
+      <c r="H17" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I17" s="1">
+        <v>3</v>
+      </c>
+      <c r="J17" s="8" t="s">
+        <v>127</v>
+      </c>
       <c r="K17" s="8"/>
       <c r="L17" s="8"/>
       <c r="M17" s="8"/>
@@ -1176,17 +1366,25 @@
       <c r="Q17" s="8"/>
       <c r="R17" s="8"/>
       <c r="S17" s="8"/>
-    </row>
-    <row r="18" spans="4:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T17" s="8"/>
+      <c r="U17" s="8"/>
+    </row>
+    <row r="18" spans="4:21" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
         <v>11</v>
       </c>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
+      <c r="H18" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="I18" s="1">
+        <v>3</v>
+      </c>
+      <c r="J18" s="8" t="s">
+        <v>128</v>
+      </c>
       <c r="K18" s="8"/>
       <c r="L18" s="8"/>
       <c r="M18" s="8"/>
@@ -1196,17 +1394,25 @@
       <c r="Q18" s="8"/>
       <c r="R18" s="8"/>
       <c r="S18" s="8"/>
-    </row>
-    <row r="19" spans="4:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T18" s="8"/>
+      <c r="U18" s="8"/>
+    </row>
+    <row r="19" spans="4:21" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
         <v>12</v>
       </c>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
       <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
+      <c r="H19" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I19" s="1">
+        <v>3</v>
+      </c>
+      <c r="J19" s="8" t="s">
+        <v>129</v>
+      </c>
       <c r="K19" s="8"/>
       <c r="L19" s="8"/>
       <c r="M19" s="8"/>
@@ -1216,17 +1422,25 @@
       <c r="Q19" s="8"/>
       <c r="R19" s="8"/>
       <c r="S19" s="8"/>
-    </row>
-    <row r="20" spans="4:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T19" s="8"/>
+      <c r="U19" s="8"/>
+    </row>
+    <row r="20" spans="4:21" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
         <v>13</v>
       </c>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
+      <c r="H20" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I20" s="1">
+        <v>2</v>
+      </c>
+      <c r="J20" s="8" t="s">
+        <v>130</v>
+      </c>
       <c r="K20" s="8"/>
       <c r="L20" s="8"/>
       <c r="M20" s="8"/>
@@ -1236,17 +1450,25 @@
       <c r="Q20" s="8"/>
       <c r="R20" s="8"/>
       <c r="S20" s="8"/>
-    </row>
-    <row r="21" spans="4:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T20" s="8"/>
+      <c r="U20" s="8"/>
+    </row>
+    <row r="21" spans="4:21" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
         <v>14</v>
       </c>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8"/>
+      <c r="H21" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I21" s="1">
+        <v>1</v>
+      </c>
+      <c r="J21" s="8" t="s">
+        <v>131</v>
+      </c>
       <c r="K21" s="8"/>
       <c r="L21" s="8"/>
       <c r="M21" s="8"/>
@@ -1256,17 +1478,25 @@
       <c r="Q21" s="8"/>
       <c r="R21" s="8"/>
       <c r="S21" s="8"/>
-    </row>
-    <row r="22" spans="4:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T21" s="8"/>
+      <c r="U21" s="8"/>
+    </row>
+    <row r="22" spans="4:21" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
         <v>15</v>
       </c>
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
+      <c r="H22" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="I22" s="1">
+        <v>0</v>
+      </c>
+      <c r="J22" s="8" t="s">
+        <v>132</v>
+      </c>
       <c r="K22" s="8"/>
       <c r="L22" s="8"/>
       <c r="M22" s="8"/>
@@ -1276,17 +1506,25 @@
       <c r="Q22" s="8"/>
       <c r="R22" s="8"/>
       <c r="S22" s="8"/>
-    </row>
-    <row r="23" spans="4:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T22" s="8"/>
+      <c r="U22" s="8"/>
+    </row>
+    <row r="23" spans="4:21" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
         <v>16</v>
       </c>
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
       <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="8"/>
+      <c r="H23" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I23" s="1">
+        <v>1</v>
+      </c>
+      <c r="J23" s="8" t="s">
+        <v>133</v>
+      </c>
       <c r="K23" s="8"/>
       <c r="L23" s="8"/>
       <c r="M23" s="8"/>
@@ -1296,17 +1534,25 @@
       <c r="Q23" s="8"/>
       <c r="R23" s="8"/>
       <c r="S23" s="8"/>
-    </row>
-    <row r="24" spans="4:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T23" s="8"/>
+      <c r="U23" s="8"/>
+    </row>
+    <row r="24" spans="4:21" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
         <v>17</v>
       </c>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
       <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8"/>
+      <c r="H24" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I24" s="1">
+        <v>2</v>
+      </c>
+      <c r="J24" s="8" t="s">
+        <v>134</v>
+      </c>
       <c r="K24" s="8"/>
       <c r="L24" s="8"/>
       <c r="M24" s="8"/>
@@ -1316,17 +1562,25 @@
       <c r="Q24" s="8"/>
       <c r="R24" s="8"/>
       <c r="S24" s="8"/>
-    </row>
-    <row r="25" spans="4:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T24" s="8"/>
+      <c r="U24" s="8"/>
+    </row>
+    <row r="25" spans="4:21" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
         <v>18</v>
       </c>
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
       <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
+      <c r="H25" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="I25" s="1">
+        <v>1</v>
+      </c>
+      <c r="J25" s="8" t="s">
+        <v>135</v>
+      </c>
       <c r="K25" s="8"/>
       <c r="L25" s="8"/>
       <c r="M25" s="8"/>
@@ -1336,17 +1590,25 @@
       <c r="Q25" s="8"/>
       <c r="R25" s="8"/>
       <c r="S25" s="8"/>
-    </row>
-    <row r="26" spans="4:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T25" s="8"/>
+      <c r="U25" s="8"/>
+    </row>
+    <row r="26" spans="4:21" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
         <v>19</v>
       </c>
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
       <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
+      <c r="H26" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="I26" s="1">
+        <v>-2</v>
+      </c>
+      <c r="J26" s="8" t="s">
+        <v>136</v>
+      </c>
       <c r="K26" s="8"/>
       <c r="L26" s="8"/>
       <c r="M26" s="8"/>
@@ -1356,17 +1618,25 @@
       <c r="Q26" s="8"/>
       <c r="R26" s="8"/>
       <c r="S26" s="8"/>
-    </row>
-    <row r="27" spans="4:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T26" s="8"/>
+      <c r="U26" s="8"/>
+    </row>
+    <row r="27" spans="4:21" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D27" t="s">
         <v>20</v>
       </c>
       <c r="E27" s="8"/>
       <c r="F27" s="8"/>
       <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="8"/>
+      <c r="H27" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="I27" s="1">
+        <v>0</v>
+      </c>
+      <c r="J27" s="8" t="s">
+        <v>137</v>
+      </c>
       <c r="K27" s="8"/>
       <c r="L27" s="8"/>
       <c r="M27" s="8"/>
@@ -1376,17 +1646,23 @@
       <c r="Q27" s="8"/>
       <c r="R27" s="8"/>
       <c r="S27" s="8"/>
-    </row>
-    <row r="28" spans="4:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T27" s="8"/>
+      <c r="U27" s="8"/>
+    </row>
+    <row r="28" spans="4:21" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
         <v>21</v>
       </c>
       <c r="E28" s="8"/>
       <c r="F28" s="8"/>
       <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
+      <c r="H28" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I28" s="1"/>
+      <c r="J28" s="8" t="s">
+        <v>138</v>
+      </c>
       <c r="K28" s="8"/>
       <c r="L28" s="8"/>
       <c r="M28" s="8"/>
@@ -1396,17 +1672,23 @@
       <c r="Q28" s="8"/>
       <c r="R28" s="8"/>
       <c r="S28" s="8"/>
-    </row>
-    <row r="29" spans="4:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T28" s="8"/>
+      <c r="U28" s="8"/>
+    </row>
+    <row r="29" spans="4:21" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D29" t="s">
         <v>22</v>
       </c>
       <c r="E29" s="8"/>
       <c r="F29" s="8"/>
       <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
+      <c r="H29" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I29" s="1"/>
+      <c r="J29" s="8" t="s">
+        <v>139</v>
+      </c>
       <c r="K29" s="8"/>
       <c r="L29" s="8"/>
       <c r="M29" s="8"/>
@@ -1416,16 +1698,18 @@
       <c r="Q29" s="8"/>
       <c r="R29" s="8"/>
       <c r="S29" s="8"/>
-    </row>
-    <row r="30" spans="4:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T29" s="8"/>
+      <c r="U29" s="8"/>
+    </row>
+    <row r="30" spans="4:21" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D30" t="s">
         <v>23</v>
       </c>
       <c r="E30" s="8"/>
       <c r="F30" s="8"/>
       <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
       <c r="J30" s="8"/>
       <c r="K30" s="8"/>
       <c r="L30" s="8"/>
@@ -1436,16 +1720,18 @@
       <c r="Q30" s="8"/>
       <c r="R30" s="8"/>
       <c r="S30" s="8"/>
-    </row>
-    <row r="31" spans="4:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T30" s="8"/>
+      <c r="U30" s="8"/>
+    </row>
+    <row r="31" spans="4:21" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D31" t="s">
         <v>24</v>
       </c>
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
       <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
       <c r="J31" s="8"/>
       <c r="K31" s="8"/>
       <c r="L31" s="8"/>
@@ -1456,16 +1742,18 @@
       <c r="Q31" s="8"/>
       <c r="R31" s="8"/>
       <c r="S31" s="8"/>
-    </row>
-    <row r="32" spans="4:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T31" s="8"/>
+      <c r="U31" s="8"/>
+    </row>
+    <row r="32" spans="4:21" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
         <v>25</v>
       </c>
       <c r="E32" s="8"/>
       <c r="F32" s="8"/>
       <c r="G32" s="8"/>
-      <c r="H32" s="8"/>
-      <c r="I32" s="8"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
       <c r="J32" s="8"/>
       <c r="K32" s="8"/>
       <c r="L32" s="8"/>
@@ -1476,16 +1764,18 @@
       <c r="Q32" s="8"/>
       <c r="R32" s="8"/>
       <c r="S32" s="8"/>
-    </row>
-    <row r="33" spans="4:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T32" s="8"/>
+      <c r="U32" s="8"/>
+    </row>
+    <row r="33" spans="4:21" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
         <v>26</v>
       </c>
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
       <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="8"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
       <c r="J33" s="8"/>
       <c r="K33" s="8"/>
       <c r="L33" s="8"/>
@@ -1496,16 +1786,18 @@
       <c r="Q33" s="8"/>
       <c r="R33" s="8"/>
       <c r="S33" s="8"/>
-    </row>
-    <row r="34" spans="4:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T33" s="8"/>
+      <c r="U33" s="8"/>
+    </row>
+    <row r="34" spans="4:21" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
         <v>27</v>
       </c>
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
       <c r="G34" s="8"/>
-      <c r="H34" s="8"/>
-      <c r="I34" s="8"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
       <c r="J34" s="8"/>
       <c r="K34" s="8"/>
       <c r="L34" s="8"/>
@@ -1516,16 +1808,18 @@
       <c r="Q34" s="8"/>
       <c r="R34" s="8"/>
       <c r="S34" s="8"/>
-    </row>
-    <row r="35" spans="4:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T34" s="8"/>
+      <c r="U34" s="8"/>
+    </row>
+    <row r="35" spans="4:21" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
         <v>28</v>
       </c>
       <c r="E35" s="8"/>
       <c r="F35" s="8"/>
       <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
-      <c r="I35" s="8"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
       <c r="J35" s="8"/>
       <c r="K35" s="8"/>
       <c r="L35" s="8"/>
@@ -1536,16 +1830,18 @@
       <c r="Q35" s="8"/>
       <c r="R35" s="8"/>
       <c r="S35" s="8"/>
-    </row>
-    <row r="36" spans="4:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T35" s="8"/>
+      <c r="U35" s="8"/>
+    </row>
+    <row r="36" spans="4:21" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
         <v>29</v>
       </c>
       <c r="E36" s="8"/>
       <c r="F36" s="8"/>
       <c r="G36" s="8"/>
-      <c r="H36" s="8"/>
-      <c r="I36" s="8"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
       <c r="J36" s="8"/>
       <c r="K36" s="8"/>
       <c r="L36" s="8"/>
@@ -1556,16 +1852,18 @@
       <c r="Q36" s="8"/>
       <c r="R36" s="8"/>
       <c r="S36" s="8"/>
-    </row>
-    <row r="37" spans="4:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T36" s="8"/>
+      <c r="U36" s="8"/>
+    </row>
+    <row r="37" spans="4:21" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
         <v>30</v>
       </c>
       <c r="E37" s="8"/>
       <c r="F37" s="8"/>
       <c r="G37" s="8"/>
-      <c r="H37" s="8"/>
-      <c r="I37" s="8"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
       <c r="J37" s="8"/>
       <c r="K37" s="8"/>
       <c r="L37" s="8"/>
@@ -1576,16 +1874,18 @@
       <c r="Q37" s="8"/>
       <c r="R37" s="8"/>
       <c r="S37" s="8"/>
-    </row>
-    <row r="38" spans="4:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T37" s="8"/>
+      <c r="U37" s="8"/>
+    </row>
+    <row r="38" spans="4:21" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
         <v>31</v>
       </c>
       <c r="E38" s="8"/>
       <c r="F38" s="8"/>
       <c r="G38" s="8"/>
-      <c r="H38" s="8"/>
-      <c r="I38" s="8"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
       <c r="J38" s="8"/>
       <c r="K38" s="8"/>
       <c r="L38" s="8"/>
@@ -1596,16 +1896,18 @@
       <c r="Q38" s="8"/>
       <c r="R38" s="8"/>
       <c r="S38" s="8"/>
-    </row>
-    <row r="39" spans="4:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T38" s="8"/>
+      <c r="U38" s="8"/>
+    </row>
+    <row r="39" spans="4:21" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
         <v>32</v>
       </c>
       <c r="E39" s="8"/>
       <c r="F39" s="8"/>
       <c r="G39" s="8"/>
-      <c r="H39" s="8"/>
-      <c r="I39" s="8"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
       <c r="J39" s="8"/>
       <c r="K39" s="8"/>
       <c r="L39" s="8"/>
@@ -1616,16 +1918,18 @@
       <c r="Q39" s="8"/>
       <c r="R39" s="8"/>
       <c r="S39" s="8"/>
-    </row>
-    <row r="40" spans="4:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T39" s="8"/>
+      <c r="U39" s="8"/>
+    </row>
+    <row r="40" spans="4:21" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
         <v>33</v>
       </c>
       <c r="E40" s="8"/>
       <c r="F40" s="8"/>
       <c r="G40" s="8"/>
-      <c r="H40" s="8"/>
-      <c r="I40" s="8"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
       <c r="J40" s="8"/>
       <c r="K40" s="8"/>
       <c r="L40" s="8"/>
@@ -1636,16 +1940,18 @@
       <c r="Q40" s="8"/>
       <c r="R40" s="8"/>
       <c r="S40" s="8"/>
-    </row>
-    <row r="41" spans="4:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T40" s="8"/>
+      <c r="U40" s="8"/>
+    </row>
+    <row r="41" spans="4:21" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
         <v>34</v>
       </c>
       <c r="E41" s="8"/>
       <c r="F41" s="8"/>
       <c r="G41" s="8"/>
-      <c r="H41" s="8"/>
-      <c r="I41" s="8"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
       <c r="J41" s="8"/>
       <c r="K41" s="8"/>
       <c r="L41" s="8"/>
@@ -1656,16 +1962,18 @@
       <c r="Q41" s="8"/>
       <c r="R41" s="8"/>
       <c r="S41" s="8"/>
-    </row>
-    <row r="42" spans="4:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T41" s="8"/>
+      <c r="U41" s="8"/>
+    </row>
+    <row r="42" spans="4:21" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D42" t="s">
         <v>35</v>
       </c>
       <c r="E42" s="8"/>
       <c r="F42" s="8"/>
       <c r="G42" s="8"/>
-      <c r="H42" s="8"/>
-      <c r="I42" s="8"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
       <c r="J42" s="8"/>
       <c r="K42" s="8"/>
       <c r="L42" s="8"/>
@@ -1676,16 +1984,18 @@
       <c r="Q42" s="8"/>
       <c r="R42" s="8"/>
       <c r="S42" s="8"/>
-    </row>
-    <row r="43" spans="4:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T42" s="8"/>
+      <c r="U42" s="8"/>
+    </row>
+    <row r="43" spans="4:21" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D43" t="s">
         <v>36</v>
       </c>
       <c r="E43" s="8"/>
       <c r="F43" s="8"/>
       <c r="G43" s="8"/>
-      <c r="H43" s="8"/>
-      <c r="I43" s="8"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
       <c r="J43" s="8"/>
       <c r="K43" s="8"/>
       <c r="L43" s="8"/>
@@ -1696,16 +2006,18 @@
       <c r="Q43" s="8"/>
       <c r="R43" s="8"/>
       <c r="S43" s="8"/>
-    </row>
-    <row r="44" spans="4:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T43" s="8"/>
+      <c r="U43" s="8"/>
+    </row>
+    <row r="44" spans="4:21" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D44" t="s">
         <v>37</v>
       </c>
       <c r="E44" s="8"/>
       <c r="F44" s="8"/>
       <c r="G44" s="8"/>
-      <c r="H44" s="8"/>
-      <c r="I44" s="8"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
       <c r="J44" s="8"/>
       <c r="K44" s="8"/>
       <c r="L44" s="8"/>
@@ -1716,16 +2028,18 @@
       <c r="Q44" s="8"/>
       <c r="R44" s="8"/>
       <c r="S44" s="8"/>
-    </row>
-    <row r="45" spans="4:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T44" s="8"/>
+      <c r="U44" s="8"/>
+    </row>
+    <row r="45" spans="4:21" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D45" t="s">
         <v>38</v>
       </c>
       <c r="E45" s="8"/>
       <c r="F45" s="8"/>
       <c r="G45" s="8"/>
-      <c r="H45" s="8"/>
-      <c r="I45" s="8"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
       <c r="J45" s="8"/>
       <c r="K45" s="8"/>
       <c r="L45" s="8"/>
@@ -1736,16 +2050,18 @@
       <c r="Q45" s="8"/>
       <c r="R45" s="8"/>
       <c r="S45" s="8"/>
-    </row>
-    <row r="46" spans="4:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T45" s="8"/>
+      <c r="U45" s="8"/>
+    </row>
+    <row r="46" spans="4:21" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D46" t="s">
         <v>39</v>
       </c>
       <c r="E46" s="8"/>
       <c r="F46" s="8"/>
       <c r="G46" s="8"/>
-      <c r="H46" s="8"/>
-      <c r="I46" s="8"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
       <c r="J46" s="8"/>
       <c r="K46" s="8"/>
       <c r="L46" s="8"/>
@@ -1756,16 +2072,18 @@
       <c r="Q46" s="8"/>
       <c r="R46" s="8"/>
       <c r="S46" s="8"/>
-    </row>
-    <row r="47" spans="4:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T46" s="8"/>
+      <c r="U46" s="8"/>
+    </row>
+    <row r="47" spans="4:21" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D47" t="s">
         <v>40</v>
       </c>
       <c r="E47" s="8"/>
       <c r="F47" s="8"/>
       <c r="G47" s="8"/>
-      <c r="H47" s="8"/>
-      <c r="I47" s="8"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
       <c r="J47" s="8"/>
       <c r="K47" s="8"/>
       <c r="L47" s="8"/>
@@ -1776,16 +2094,18 @@
       <c r="Q47" s="8"/>
       <c r="R47" s="8"/>
       <c r="S47" s="8"/>
-    </row>
-    <row r="48" spans="4:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T47" s="8"/>
+      <c r="U47" s="8"/>
+    </row>
+    <row r="48" spans="4:21" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D48" t="s">
         <v>41</v>
       </c>
       <c r="E48" s="8"/>
       <c r="F48" s="8"/>
       <c r="G48" s="8"/>
-      <c r="H48" s="8"/>
-      <c r="I48" s="8"/>
+      <c r="H48" s="1"/>
+      <c r="I48" s="1"/>
       <c r="J48" s="8"/>
       <c r="K48" s="8"/>
       <c r="L48" s="8"/>
@@ -1796,16 +2116,18 @@
       <c r="Q48" s="8"/>
       <c r="R48" s="8"/>
       <c r="S48" s="8"/>
-    </row>
-    <row r="49" spans="4:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T48" s="8"/>
+      <c r="U48" s="8"/>
+    </row>
+    <row r="49" spans="4:21" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D49" t="s">
         <v>42</v>
       </c>
       <c r="E49" s="8"/>
       <c r="F49" s="8"/>
       <c r="G49" s="8"/>
-      <c r="H49" s="8"/>
-      <c r="I49" s="8"/>
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
       <c r="J49" s="8"/>
       <c r="K49" s="8"/>
       <c r="L49" s="8"/>
@@ -1816,16 +2138,18 @@
       <c r="Q49" s="8"/>
       <c r="R49" s="8"/>
       <c r="S49" s="8"/>
-    </row>
-    <row r="50" spans="4:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T49" s="8"/>
+      <c r="U49" s="8"/>
+    </row>
+    <row r="50" spans="4:21" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D50" t="s">
         <v>43</v>
       </c>
       <c r="E50" s="8"/>
       <c r="F50" s="8"/>
       <c r="G50" s="8"/>
-      <c r="H50" s="8"/>
-      <c r="I50" s="8"/>
+      <c r="H50" s="1"/>
+      <c r="I50" s="1"/>
       <c r="J50" s="8"/>
       <c r="K50" s="8"/>
       <c r="L50" s="8"/>
@@ -1836,16 +2160,18 @@
       <c r="Q50" s="8"/>
       <c r="R50" s="8"/>
       <c r="S50" s="8"/>
-    </row>
-    <row r="51" spans="4:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T50" s="8"/>
+      <c r="U50" s="8"/>
+    </row>
+    <row r="51" spans="4:21" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D51" t="s">
         <v>44</v>
       </c>
       <c r="E51" s="8"/>
       <c r="F51" s="8"/>
       <c r="G51" s="8"/>
-      <c r="H51" s="8"/>
-      <c r="I51" s="8"/>
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
       <c r="J51" s="8"/>
       <c r="K51" s="8"/>
       <c r="L51" s="8"/>
@@ -1856,16 +2182,18 @@
       <c r="Q51" s="8"/>
       <c r="R51" s="8"/>
       <c r="S51" s="8"/>
-    </row>
-    <row r="52" spans="4:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T51" s="8"/>
+      <c r="U51" s="8"/>
+    </row>
+    <row r="52" spans="4:21" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D52" t="s">
         <v>45</v>
       </c>
       <c r="E52" s="8"/>
       <c r="F52" s="8"/>
       <c r="G52" s="8"/>
-      <c r="H52" s="8"/>
-      <c r="I52" s="8"/>
+      <c r="H52" s="1"/>
+      <c r="I52" s="1"/>
       <c r="J52" s="8"/>
       <c r="K52" s="8"/>
       <c r="L52" s="8"/>
@@ -1876,16 +2204,18 @@
       <c r="Q52" s="8"/>
       <c r="R52" s="8"/>
       <c r="S52" s="8"/>
-    </row>
-    <row r="53" spans="4:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T52" s="8"/>
+      <c r="U52" s="8"/>
+    </row>
+    <row r="53" spans="4:21" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D53" t="s">
         <v>46</v>
       </c>
       <c r="E53" s="8"/>
       <c r="F53" s="8"/>
       <c r="G53" s="8"/>
-      <c r="H53" s="8"/>
-      <c r="I53" s="8"/>
+      <c r="H53" s="1"/>
+      <c r="I53" s="1"/>
       <c r="J53" s="8"/>
       <c r="K53" s="8"/>
       <c r="L53" s="8"/>
@@ -1896,16 +2226,18 @@
       <c r="Q53" s="8"/>
       <c r="R53" s="8"/>
       <c r="S53" s="8"/>
-    </row>
-    <row r="54" spans="4:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T53" s="8"/>
+      <c r="U53" s="8"/>
+    </row>
+    <row r="54" spans="4:21" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D54" t="s">
         <v>47</v>
       </c>
       <c r="E54" s="8"/>
       <c r="F54" s="8"/>
       <c r="G54" s="8"/>
-      <c r="H54" s="8"/>
-      <c r="I54" s="8"/>
+      <c r="H54" s="1"/>
+      <c r="I54" s="1"/>
       <c r="J54" s="8"/>
       <c r="K54" s="8"/>
       <c r="L54" s="8"/>
@@ -1916,16 +2248,18 @@
       <c r="Q54" s="8"/>
       <c r="R54" s="8"/>
       <c r="S54" s="8"/>
-    </row>
-    <row r="55" spans="4:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T54" s="8"/>
+      <c r="U54" s="8"/>
+    </row>
+    <row r="55" spans="4:21" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D55" t="s">
         <v>48</v>
       </c>
       <c r="E55" s="8"/>
       <c r="F55" s="8"/>
       <c r="G55" s="8"/>
-      <c r="H55" s="8"/>
-      <c r="I55" s="8"/>
+      <c r="H55" s="1"/>
+      <c r="I55" s="1"/>
       <c r="J55" s="8"/>
       <c r="K55" s="8"/>
       <c r="L55" s="8"/>
@@ -1936,16 +2270,18 @@
       <c r="Q55" s="8"/>
       <c r="R55" s="8"/>
       <c r="S55" s="8"/>
-    </row>
-    <row r="56" spans="4:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T55" s="8"/>
+      <c r="U55" s="8"/>
+    </row>
+    <row r="56" spans="4:21" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D56" t="s">
         <v>49</v>
       </c>
       <c r="E56" s="8"/>
       <c r="F56" s="8"/>
       <c r="G56" s="8"/>
-      <c r="H56" s="8"/>
-      <c r="I56" s="8"/>
+      <c r="H56" s="1"/>
+      <c r="I56" s="1"/>
       <c r="J56" s="8"/>
       <c r="K56" s="8"/>
       <c r="L56" s="8"/>
@@ -1956,16 +2292,18 @@
       <c r="Q56" s="8"/>
       <c r="R56" s="8"/>
       <c r="S56" s="8"/>
-    </row>
-    <row r="57" spans="4:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T56" s="8"/>
+      <c r="U56" s="8"/>
+    </row>
+    <row r="57" spans="4:21" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D57" t="s">
         <v>50</v>
       </c>
       <c r="E57" s="8"/>
       <c r="F57" s="8"/>
       <c r="G57" s="8"/>
-      <c r="H57" s="8"/>
-      <c r="I57" s="8"/>
+      <c r="H57" s="1"/>
+      <c r="I57" s="1"/>
       <c r="J57" s="8"/>
       <c r="K57" s="8"/>
       <c r="L57" s="8"/>
@@ -1976,16 +2314,18 @@
       <c r="Q57" s="8"/>
       <c r="R57" s="8"/>
       <c r="S57" s="8"/>
-    </row>
-    <row r="58" spans="4:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T57" s="8"/>
+      <c r="U57" s="8"/>
+    </row>
+    <row r="58" spans="4:21" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D58" t="s">
         <v>51</v>
       </c>
       <c r="E58" s="8"/>
       <c r="F58" s="8"/>
       <c r="G58" s="8"/>
-      <c r="H58" s="8"/>
-      <c r="I58" s="8"/>
+      <c r="H58" s="1"/>
+      <c r="I58" s="1"/>
       <c r="J58" s="8"/>
       <c r="K58" s="8"/>
       <c r="L58" s="8"/>
@@ -1996,16 +2336,18 @@
       <c r="Q58" s="8"/>
       <c r="R58" s="8"/>
       <c r="S58" s="8"/>
-    </row>
-    <row r="59" spans="4:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T58" s="8"/>
+      <c r="U58" s="8"/>
+    </row>
+    <row r="59" spans="4:21" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D59" t="s">
         <v>52</v>
       </c>
       <c r="E59" s="8"/>
       <c r="F59" s="8"/>
       <c r="G59" s="8"/>
-      <c r="H59" s="8"/>
-      <c r="I59" s="8"/>
+      <c r="H59" s="1"/>
+      <c r="I59" s="1"/>
       <c r="J59" s="8"/>
       <c r="K59" s="8"/>
       <c r="L59" s="8"/>
@@ -2016,16 +2358,18 @@
       <c r="Q59" s="8"/>
       <c r="R59" s="8"/>
       <c r="S59" s="8"/>
-    </row>
-    <row r="60" spans="4:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T59" s="8"/>
+      <c r="U59" s="8"/>
+    </row>
+    <row r="60" spans="4:21" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D60" t="s">
         <v>53</v>
       </c>
       <c r="E60" s="8"/>
       <c r="F60" s="8"/>
       <c r="G60" s="8"/>
-      <c r="H60" s="8"/>
-      <c r="I60" s="8"/>
+      <c r="H60" s="1"/>
+      <c r="I60" s="1"/>
       <c r="J60" s="8"/>
       <c r="K60" s="8"/>
       <c r="L60" s="8"/>
@@ -2036,16 +2380,18 @@
       <c r="Q60" s="8"/>
       <c r="R60" s="8"/>
       <c r="S60" s="8"/>
-    </row>
-    <row r="61" spans="4:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T60" s="8"/>
+      <c r="U60" s="8"/>
+    </row>
+    <row r="61" spans="4:21" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D61" t="s">
         <v>54</v>
       </c>
       <c r="E61" s="8"/>
       <c r="F61" s="8"/>
       <c r="G61" s="8"/>
-      <c r="H61" s="8"/>
-      <c r="I61" s="8"/>
+      <c r="H61" s="1"/>
+      <c r="I61" s="1"/>
       <c r="J61" s="8"/>
       <c r="K61" s="8"/>
       <c r="L61" s="8"/>
@@ -2056,16 +2402,18 @@
       <c r="Q61" s="8"/>
       <c r="R61" s="8"/>
       <c r="S61" s="8"/>
-    </row>
-    <row r="62" spans="4:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T61" s="8"/>
+      <c r="U61" s="8"/>
+    </row>
+    <row r="62" spans="4:21" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D62" t="s">
         <v>55</v>
       </c>
       <c r="E62" s="8"/>
       <c r="F62" s="8"/>
       <c r="G62" s="8"/>
-      <c r="H62" s="8"/>
-      <c r="I62" s="8"/>
+      <c r="H62" s="1"/>
+      <c r="I62" s="1"/>
       <c r="J62" s="8"/>
       <c r="K62" s="8"/>
       <c r="L62" s="8"/>
@@ -2076,16 +2424,18 @@
       <c r="Q62" s="8"/>
       <c r="R62" s="8"/>
       <c r="S62" s="8"/>
-    </row>
-    <row r="63" spans="4:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T62" s="8"/>
+      <c r="U62" s="8"/>
+    </row>
+    <row r="63" spans="4:21" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D63" t="s">
         <v>56</v>
       </c>
       <c r="E63" s="8"/>
       <c r="F63" s="8"/>
       <c r="G63" s="8"/>
-      <c r="H63" s="8"/>
-      <c r="I63" s="8"/>
+      <c r="H63" s="1"/>
+      <c r="I63" s="1"/>
       <c r="J63" s="8"/>
       <c r="K63" s="8"/>
       <c r="L63" s="8"/>
@@ -2096,16 +2446,18 @@
       <c r="Q63" s="8"/>
       <c r="R63" s="8"/>
       <c r="S63" s="8"/>
-    </row>
-    <row r="64" spans="4:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T63" s="8"/>
+      <c r="U63" s="8"/>
+    </row>
+    <row r="64" spans="4:21" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D64" t="s">
         <v>57</v>
       </c>
       <c r="E64" s="8"/>
       <c r="F64" s="8"/>
       <c r="G64" s="8"/>
-      <c r="H64" s="8"/>
-      <c r="I64" s="8"/>
+      <c r="H64" s="1"/>
+      <c r="I64" s="1"/>
       <c r="J64" s="8"/>
       <c r="K64" s="8"/>
       <c r="L64" s="8"/>
@@ -2116,16 +2468,18 @@
       <c r="Q64" s="8"/>
       <c r="R64" s="8"/>
       <c r="S64" s="8"/>
-    </row>
-    <row r="65" spans="4:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T64" s="8"/>
+      <c r="U64" s="8"/>
+    </row>
+    <row r="65" spans="4:21" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D65" t="s">
         <v>58</v>
       </c>
       <c r="E65" s="8"/>
       <c r="F65" s="8"/>
       <c r="G65" s="8"/>
-      <c r="H65" s="8"/>
-      <c r="I65" s="8"/>
+      <c r="H65" s="1"/>
+      <c r="I65" s="1"/>
       <c r="J65" s="8"/>
       <c r="K65" s="8"/>
       <c r="L65" s="8"/>
@@ -2136,16 +2490,18 @@
       <c r="Q65" s="8"/>
       <c r="R65" s="8"/>
       <c r="S65" s="8"/>
-    </row>
-    <row r="66" spans="4:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T65" s="8"/>
+      <c r="U65" s="8"/>
+    </row>
+    <row r="66" spans="4:21" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D66" t="s">
         <v>59</v>
       </c>
       <c r="E66" s="8"/>
       <c r="F66" s="8"/>
       <c r="G66" s="8"/>
-      <c r="H66" s="8"/>
-      <c r="I66" s="8"/>
+      <c r="H66" s="1"/>
+      <c r="I66" s="1"/>
       <c r="J66" s="8"/>
       <c r="K66" s="8"/>
       <c r="L66" s="8"/>
@@ -2156,16 +2512,18 @@
       <c r="Q66" s="8"/>
       <c r="R66" s="8"/>
       <c r="S66" s="8"/>
-    </row>
-    <row r="67" spans="4:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T66" s="8"/>
+      <c r="U66" s="8"/>
+    </row>
+    <row r="67" spans="4:21" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D67" t="s">
         <v>60</v>
       </c>
       <c r="E67" s="8"/>
       <c r="F67" s="8"/>
       <c r="G67" s="8"/>
-      <c r="H67" s="8"/>
-      <c r="I67" s="8"/>
+      <c r="H67" s="1"/>
+      <c r="I67" s="1"/>
       <c r="J67" s="8"/>
       <c r="K67" s="8"/>
       <c r="L67" s="8"/>
@@ -2176,16 +2534,18 @@
       <c r="Q67" s="8"/>
       <c r="R67" s="8"/>
       <c r="S67" s="8"/>
-    </row>
-    <row r="68" spans="4:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T67" s="8"/>
+      <c r="U67" s="8"/>
+    </row>
+    <row r="68" spans="4:21" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D68" t="s">
         <v>61</v>
       </c>
       <c r="E68" s="8"/>
       <c r="F68" s="8"/>
       <c r="G68" s="8"/>
-      <c r="H68" s="8"/>
-      <c r="I68" s="8"/>
+      <c r="H68" s="1"/>
+      <c r="I68" s="1"/>
       <c r="J68" s="8"/>
       <c r="K68" s="8"/>
       <c r="L68" s="8"/>
@@ -2196,16 +2556,18 @@
       <c r="Q68" s="8"/>
       <c r="R68" s="8"/>
       <c r="S68" s="8"/>
-    </row>
-    <row r="69" spans="4:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T68" s="8"/>
+      <c r="U68" s="8"/>
+    </row>
+    <row r="69" spans="4:21" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D69" t="s">
         <v>62</v>
       </c>
       <c r="E69" s="8"/>
       <c r="F69" s="8"/>
       <c r="G69" s="8"/>
-      <c r="H69" s="8"/>
-      <c r="I69" s="8"/>
+      <c r="H69" s="1"/>
+      <c r="I69" s="1"/>
       <c r="J69" s="8"/>
       <c r="K69" s="8"/>
       <c r="L69" s="8"/>
@@ -2216,16 +2578,18 @@
       <c r="Q69" s="8"/>
       <c r="R69" s="8"/>
       <c r="S69" s="8"/>
-    </row>
-    <row r="70" spans="4:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T69" s="8"/>
+      <c r="U69" s="8"/>
+    </row>
+    <row r="70" spans="4:21" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D70" t="s">
         <v>63</v>
       </c>
       <c r="E70" s="8"/>
       <c r="F70" s="8"/>
       <c r="G70" s="8"/>
-      <c r="H70" s="8"/>
-      <c r="I70" s="8"/>
+      <c r="H70" s="1"/>
+      <c r="I70" s="1"/>
       <c r="J70" s="8"/>
       <c r="K70" s="8"/>
       <c r="L70" s="8"/>
@@ -2236,16 +2600,18 @@
       <c r="Q70" s="8"/>
       <c r="R70" s="8"/>
       <c r="S70" s="8"/>
-    </row>
-    <row r="71" spans="4:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T70" s="8"/>
+      <c r="U70" s="8"/>
+    </row>
+    <row r="71" spans="4:21" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D71" t="s">
         <v>64</v>
       </c>
       <c r="E71" s="8"/>
       <c r="F71" s="8"/>
       <c r="G71" s="8"/>
-      <c r="H71" s="8"/>
-      <c r="I71" s="8"/>
+      <c r="H71" s="1"/>
+      <c r="I71" s="1"/>
       <c r="J71" s="8"/>
       <c r="K71" s="8"/>
       <c r="L71" s="8"/>
@@ -2256,16 +2622,18 @@
       <c r="Q71" s="8"/>
       <c r="R71" s="8"/>
       <c r="S71" s="8"/>
-    </row>
-    <row r="72" spans="4:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T71" s="8"/>
+      <c r="U71" s="8"/>
+    </row>
+    <row r="72" spans="4:21" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D72" t="s">
         <v>65</v>
       </c>
       <c r="E72" s="8"/>
       <c r="F72" s="8"/>
       <c r="G72" s="8"/>
-      <c r="H72" s="8"/>
-      <c r="I72" s="8"/>
+      <c r="H72" s="1"/>
+      <c r="I72" s="1"/>
       <c r="J72" s="8"/>
       <c r="K72" s="8"/>
       <c r="L72" s="8"/>
@@ -2276,16 +2644,18 @@
       <c r="Q72" s="8"/>
       <c r="R72" s="8"/>
       <c r="S72" s="8"/>
-    </row>
-    <row r="73" spans="4:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T72" s="8"/>
+      <c r="U72" s="8"/>
+    </row>
+    <row r="73" spans="4:21" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D73" t="s">
         <v>66</v>
       </c>
       <c r="E73" s="8"/>
       <c r="F73" s="8"/>
       <c r="G73" s="8"/>
-      <c r="H73" s="8"/>
-      <c r="I73" s="8"/>
+      <c r="H73" s="1"/>
+      <c r="I73" s="1"/>
       <c r="J73" s="8"/>
       <c r="K73" s="8"/>
       <c r="L73" s="8"/>
@@ -2296,16 +2666,18 @@
       <c r="Q73" s="8"/>
       <c r="R73" s="8"/>
       <c r="S73" s="8"/>
-    </row>
-    <row r="74" spans="4:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T73" s="8"/>
+      <c r="U73" s="8"/>
+    </row>
+    <row r="74" spans="4:21" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D74" t="s">
         <v>67</v>
       </c>
       <c r="E74" s="8"/>
       <c r="F74" s="8"/>
       <c r="G74" s="8"/>
-      <c r="H74" s="8"/>
-      <c r="I74" s="8"/>
+      <c r="H74" s="1"/>
+      <c r="I74" s="1"/>
       <c r="J74" s="8"/>
       <c r="K74" s="8"/>
       <c r="L74" s="8"/>
@@ -2316,16 +2688,18 @@
       <c r="Q74" s="8"/>
       <c r="R74" s="8"/>
       <c r="S74" s="8"/>
-    </row>
-    <row r="75" spans="4:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T74" s="8"/>
+      <c r="U74" s="8"/>
+    </row>
+    <row r="75" spans="4:21" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D75" t="s">
         <v>68</v>
       </c>
       <c r="E75" s="8"/>
       <c r="F75" s="8"/>
       <c r="G75" s="8"/>
-      <c r="H75" s="8"/>
-      <c r="I75" s="8"/>
+      <c r="H75" s="1"/>
+      <c r="I75" s="1"/>
       <c r="J75" s="8"/>
       <c r="K75" s="8"/>
       <c r="L75" s="8"/>
@@ -2336,16 +2710,18 @@
       <c r="Q75" s="8"/>
       <c r="R75" s="8"/>
       <c r="S75" s="8"/>
-    </row>
-    <row r="76" spans="4:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T75" s="8"/>
+      <c r="U75" s="8"/>
+    </row>
+    <row r="76" spans="4:21" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D76" t="s">
         <v>69</v>
       </c>
       <c r="E76" s="8"/>
       <c r="F76" s="8"/>
       <c r="G76" s="8"/>
-      <c r="H76" s="8"/>
-      <c r="I76" s="8"/>
+      <c r="H76" s="1"/>
+      <c r="I76" s="1"/>
       <c r="J76" s="8"/>
       <c r="K76" s="8"/>
       <c r="L76" s="8"/>
@@ -2356,16 +2732,18 @@
       <c r="Q76" s="8"/>
       <c r="R76" s="8"/>
       <c r="S76" s="8"/>
-    </row>
-    <row r="77" spans="4:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T76" s="8"/>
+      <c r="U76" s="8"/>
+    </row>
+    <row r="77" spans="4:21" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D77" t="s">
         <v>70</v>
       </c>
       <c r="E77" s="8"/>
       <c r="F77" s="8"/>
       <c r="G77" s="8"/>
-      <c r="H77" s="8"/>
-      <c r="I77" s="8"/>
+      <c r="H77" s="1"/>
+      <c r="I77" s="1"/>
       <c r="J77" s="8"/>
       <c r="K77" s="8"/>
       <c r="L77" s="8"/>
@@ -2376,16 +2754,18 @@
       <c r="Q77" s="8"/>
       <c r="R77" s="8"/>
       <c r="S77" s="8"/>
-    </row>
-    <row r="78" spans="4:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T77" s="8"/>
+      <c r="U77" s="8"/>
+    </row>
+    <row r="78" spans="4:21" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D78" t="s">
         <v>71</v>
       </c>
       <c r="E78" s="8"/>
       <c r="F78" s="8"/>
       <c r="G78" s="8"/>
-      <c r="H78" s="8"/>
-      <c r="I78" s="8"/>
+      <c r="H78" s="1"/>
+      <c r="I78" s="1"/>
       <c r="J78" s="8"/>
       <c r="K78" s="8"/>
       <c r="L78" s="8"/>
@@ -2396,16 +2776,18 @@
       <c r="Q78" s="8"/>
       <c r="R78" s="8"/>
       <c r="S78" s="8"/>
-    </row>
-    <row r="79" spans="4:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T78" s="8"/>
+      <c r="U78" s="8"/>
+    </row>
+    <row r="79" spans="4:21" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D79" t="s">
         <v>72</v>
       </c>
       <c r="E79" s="8"/>
       <c r="F79" s="8"/>
       <c r="G79" s="8"/>
-      <c r="H79" s="8"/>
-      <c r="I79" s="8"/>
+      <c r="H79" s="1"/>
+      <c r="I79" s="1"/>
       <c r="J79" s="8"/>
       <c r="K79" s="8"/>
       <c r="L79" s="8"/>
@@ -2416,16 +2798,18 @@
       <c r="Q79" s="8"/>
       <c r="R79" s="8"/>
       <c r="S79" s="8"/>
-    </row>
-    <row r="80" spans="4:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T79" s="8"/>
+      <c r="U79" s="8"/>
+    </row>
+    <row r="80" spans="4:21" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D80" t="s">
         <v>73</v>
       </c>
       <c r="E80" s="8"/>
       <c r="F80" s="8"/>
       <c r="G80" s="8"/>
-      <c r="H80" s="8"/>
-      <c r="I80" s="8"/>
+      <c r="H80" s="1"/>
+      <c r="I80" s="1"/>
       <c r="J80" s="8"/>
       <c r="K80" s="8"/>
       <c r="L80" s="8"/>
@@ -2436,16 +2820,18 @@
       <c r="Q80" s="8"/>
       <c r="R80" s="8"/>
       <c r="S80" s="8"/>
-    </row>
-    <row r="81" spans="4:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T80" s="8"/>
+      <c r="U80" s="8"/>
+    </row>
+    <row r="81" spans="4:21" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D81" t="s">
         <v>74</v>
       </c>
       <c r="E81" s="8"/>
       <c r="F81" s="8"/>
       <c r="G81" s="8"/>
-      <c r="H81" s="8"/>
-      <c r="I81" s="8"/>
+      <c r="H81" s="1"/>
+      <c r="I81" s="1"/>
       <c r="J81" s="8"/>
       <c r="K81" s="8"/>
       <c r="L81" s="8"/>
@@ -2456,52 +2842,60 @@
       <c r="Q81" s="8"/>
       <c r="R81" s="8"/>
       <c r="S81" s="8"/>
+      <c r="T81" s="8"/>
+      <c r="U81" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="152">
-    <mergeCell ref="H81:S81"/>
-    <mergeCell ref="H71:S71"/>
-    <mergeCell ref="H72:S72"/>
-    <mergeCell ref="H73:S73"/>
-    <mergeCell ref="H74:S74"/>
-    <mergeCell ref="H75:S75"/>
-    <mergeCell ref="H76:S76"/>
-    <mergeCell ref="H59:S59"/>
-    <mergeCell ref="H60:S60"/>
-    <mergeCell ref="H61:S61"/>
-    <mergeCell ref="H62:S62"/>
-    <mergeCell ref="H63:S63"/>
-    <mergeCell ref="H64:S64"/>
-    <mergeCell ref="H79:S79"/>
-    <mergeCell ref="H80:S80"/>
-    <mergeCell ref="H16:S16"/>
-    <mergeCell ref="H17:S17"/>
-    <mergeCell ref="H18:S18"/>
-    <mergeCell ref="H47:S47"/>
-    <mergeCell ref="H48:S48"/>
-    <mergeCell ref="H49:S49"/>
-    <mergeCell ref="H50:S50"/>
-    <mergeCell ref="H51:S51"/>
-    <mergeCell ref="H52:S52"/>
-    <mergeCell ref="H35:S35"/>
-    <mergeCell ref="H36:S36"/>
-    <mergeCell ref="H37:S37"/>
-    <mergeCell ref="H38:S38"/>
-    <mergeCell ref="H39:S39"/>
-    <mergeCell ref="H40:S40"/>
-    <mergeCell ref="H46:S46"/>
-    <mergeCell ref="H41:S41"/>
-    <mergeCell ref="H42:S42"/>
-    <mergeCell ref="H6:S6"/>
-    <mergeCell ref="H8:S8"/>
-    <mergeCell ref="H9:S9"/>
-    <mergeCell ref="H10:S10"/>
-    <mergeCell ref="H11:S11"/>
-    <mergeCell ref="H12:S12"/>
-    <mergeCell ref="H13:S13"/>
-    <mergeCell ref="H14:S14"/>
-    <mergeCell ref="H15:S15"/>
-    <mergeCell ref="H7:S7"/>
+    <mergeCell ref="J81:U81"/>
+    <mergeCell ref="J71:U71"/>
+    <mergeCell ref="J72:U72"/>
+    <mergeCell ref="J73:U73"/>
+    <mergeCell ref="J74:U74"/>
+    <mergeCell ref="J75:U75"/>
+    <mergeCell ref="J76:U76"/>
+    <mergeCell ref="J59:U59"/>
+    <mergeCell ref="J60:U60"/>
+    <mergeCell ref="J61:U61"/>
+    <mergeCell ref="J62:U62"/>
+    <mergeCell ref="J63:U63"/>
+    <mergeCell ref="J64:U64"/>
+    <mergeCell ref="J79:U79"/>
+    <mergeCell ref="J80:U80"/>
+    <mergeCell ref="J16:U16"/>
+    <mergeCell ref="J17:U17"/>
+    <mergeCell ref="J18:U18"/>
+    <mergeCell ref="J47:U47"/>
+    <mergeCell ref="J48:U48"/>
+    <mergeCell ref="J49:U49"/>
+    <mergeCell ref="J50:U50"/>
+    <mergeCell ref="J51:U51"/>
+    <mergeCell ref="J52:U52"/>
+    <mergeCell ref="J35:U35"/>
+    <mergeCell ref="J36:U36"/>
+    <mergeCell ref="J37:U37"/>
+    <mergeCell ref="J38:U38"/>
+    <mergeCell ref="J39:U39"/>
+    <mergeCell ref="J40:U40"/>
+    <mergeCell ref="J46:U46"/>
+    <mergeCell ref="J41:U41"/>
+    <mergeCell ref="J42:U42"/>
+    <mergeCell ref="J31:U31"/>
+    <mergeCell ref="J32:U32"/>
+    <mergeCell ref="J33:U33"/>
+    <mergeCell ref="J34:U34"/>
+    <mergeCell ref="J29:U29"/>
+    <mergeCell ref="J30:U30"/>
+    <mergeCell ref="J6:U6"/>
+    <mergeCell ref="J8:U8"/>
+    <mergeCell ref="J9:U9"/>
+    <mergeCell ref="J10:U10"/>
+    <mergeCell ref="J11:U11"/>
+    <mergeCell ref="J12:U12"/>
+    <mergeCell ref="J13:U13"/>
+    <mergeCell ref="J14:U14"/>
+    <mergeCell ref="J15:U15"/>
+    <mergeCell ref="J7:U7"/>
     <mergeCell ref="E81:G81"/>
     <mergeCell ref="E73:G73"/>
     <mergeCell ref="E74:G74"/>
@@ -2540,6 +2934,13 @@
     <mergeCell ref="E42:G42"/>
     <mergeCell ref="E43:G43"/>
     <mergeCell ref="E44:G44"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="E27:G27"/>
     <mergeCell ref="E6:G6"/>
     <mergeCell ref="E7:G7"/>
     <mergeCell ref="E8:G8"/>
@@ -2547,39 +2948,35 @@
     <mergeCell ref="E10:G10"/>
     <mergeCell ref="E11:G11"/>
     <mergeCell ref="E12:G12"/>
-    <mergeCell ref="H77:S77"/>
-    <mergeCell ref="H78:S78"/>
-    <mergeCell ref="H67:S67"/>
-    <mergeCell ref="H68:S68"/>
-    <mergeCell ref="H69:S69"/>
-    <mergeCell ref="H70:S70"/>
-    <mergeCell ref="H65:S65"/>
-    <mergeCell ref="H66:S66"/>
-    <mergeCell ref="H55:S55"/>
-    <mergeCell ref="H56:S56"/>
-    <mergeCell ref="H57:S57"/>
-    <mergeCell ref="H58:S58"/>
-    <mergeCell ref="H53:S53"/>
-    <mergeCell ref="H54:S54"/>
-    <mergeCell ref="H43:S43"/>
-    <mergeCell ref="H44:S44"/>
-    <mergeCell ref="H45:S45"/>
-    <mergeCell ref="H31:S31"/>
-    <mergeCell ref="H32:S32"/>
-    <mergeCell ref="H33:S33"/>
-    <mergeCell ref="H34:S34"/>
-    <mergeCell ref="H29:S29"/>
-    <mergeCell ref="H30:S30"/>
-    <mergeCell ref="H19:S19"/>
-    <mergeCell ref="H20:S20"/>
-    <mergeCell ref="H21:S21"/>
-    <mergeCell ref="H22:S22"/>
-    <mergeCell ref="H23:S23"/>
-    <mergeCell ref="H24:S24"/>
-    <mergeCell ref="H25:S25"/>
-    <mergeCell ref="H26:S26"/>
-    <mergeCell ref="H27:S27"/>
-    <mergeCell ref="H28:S28"/>
+    <mergeCell ref="J77:U77"/>
+    <mergeCell ref="J78:U78"/>
+    <mergeCell ref="J67:U67"/>
+    <mergeCell ref="J68:U68"/>
+    <mergeCell ref="J69:U69"/>
+    <mergeCell ref="J70:U70"/>
+    <mergeCell ref="J65:U65"/>
+    <mergeCell ref="J66:U66"/>
+    <mergeCell ref="J55:U55"/>
+    <mergeCell ref="J56:U56"/>
+    <mergeCell ref="J57:U57"/>
+    <mergeCell ref="J58:U58"/>
+    <mergeCell ref="J53:U53"/>
+    <mergeCell ref="J54:U54"/>
+    <mergeCell ref="J43:U43"/>
+    <mergeCell ref="J44:U44"/>
+    <mergeCell ref="J45:U45"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="J19:U19"/>
+    <mergeCell ref="J20:U20"/>
+    <mergeCell ref="J21:U21"/>
+    <mergeCell ref="J22:U22"/>
+    <mergeCell ref="J23:U23"/>
+    <mergeCell ref="J24:U24"/>
+    <mergeCell ref="J25:U25"/>
+    <mergeCell ref="J26:U26"/>
+    <mergeCell ref="J27:U27"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="J28:U28"/>
     <mergeCell ref="E57:G57"/>
     <mergeCell ref="E58:G58"/>
     <mergeCell ref="E59:G59"/>
@@ -2601,16 +2998,7 @@
     <mergeCell ref="E36:G36"/>
     <mergeCell ref="E31:G31"/>
     <mergeCell ref="E32:G32"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="E27:G27"/>
     <mergeCell ref="E28:G28"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="E30:G30"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2623,7 +3011,7 @@
   <dimension ref="F2:Z74"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L15" sqref="F2:Z15"/>
+      <selection activeCell="F9" sqref="F9:H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
update changbi and zhuxing
</commit_message>
<xml_diff>
--- a/cards.xlsx
+++ b/cards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\_projects\_OFF\theParasitized\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F524905F-D286-46B8-AAF4-AE1766FC83B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2F071DA-3478-438F-84EE-DAF67C765E5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6492" yWindow="816" windowWidth="14616" windowHeight="11340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -534,7 +534,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -562,6 +562,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -648,7 +654,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -666,6 +672,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -675,19 +693,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -972,7 +981,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="D2:AB81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B11" workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="J27" sqref="J27:U27"/>
     </sheetView>
   </sheetViews>
@@ -2847,21 +2856,119 @@
     </row>
   </sheetData>
   <mergeCells count="152">
-    <mergeCell ref="J81:U81"/>
-    <mergeCell ref="J71:U71"/>
-    <mergeCell ref="J72:U72"/>
-    <mergeCell ref="J73:U73"/>
-    <mergeCell ref="J74:U74"/>
-    <mergeCell ref="J75:U75"/>
-    <mergeCell ref="J76:U76"/>
-    <mergeCell ref="J59:U59"/>
-    <mergeCell ref="J60:U60"/>
-    <mergeCell ref="J61:U61"/>
-    <mergeCell ref="J62:U62"/>
-    <mergeCell ref="J63:U63"/>
-    <mergeCell ref="J64:U64"/>
-    <mergeCell ref="J79:U79"/>
-    <mergeCell ref="J80:U80"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="J28:U28"/>
+    <mergeCell ref="E57:G57"/>
+    <mergeCell ref="E58:G58"/>
+    <mergeCell ref="E59:G59"/>
+    <mergeCell ref="E60:G60"/>
+    <mergeCell ref="E55:G55"/>
+    <mergeCell ref="E56:G56"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="E51:G51"/>
+    <mergeCell ref="E52:G52"/>
+    <mergeCell ref="E53:G53"/>
+    <mergeCell ref="E54:G54"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="J19:U19"/>
+    <mergeCell ref="J20:U20"/>
+    <mergeCell ref="J21:U21"/>
+    <mergeCell ref="J22:U22"/>
+    <mergeCell ref="J23:U23"/>
+    <mergeCell ref="J24:U24"/>
+    <mergeCell ref="J25:U25"/>
+    <mergeCell ref="J26:U26"/>
+    <mergeCell ref="J27:U27"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="J77:U77"/>
+    <mergeCell ref="J78:U78"/>
+    <mergeCell ref="J67:U67"/>
+    <mergeCell ref="J68:U68"/>
+    <mergeCell ref="J69:U69"/>
+    <mergeCell ref="J70:U70"/>
+    <mergeCell ref="J65:U65"/>
+    <mergeCell ref="J66:U66"/>
+    <mergeCell ref="J55:U55"/>
+    <mergeCell ref="J56:U56"/>
+    <mergeCell ref="J57:U57"/>
+    <mergeCell ref="J58:U58"/>
+    <mergeCell ref="J53:U53"/>
+    <mergeCell ref="J54:U54"/>
+    <mergeCell ref="J43:U43"/>
+    <mergeCell ref="J44:U44"/>
+    <mergeCell ref="J45:U45"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="E81:G81"/>
+    <mergeCell ref="E73:G73"/>
+    <mergeCell ref="E74:G74"/>
+    <mergeCell ref="E75:G75"/>
+    <mergeCell ref="E76:G76"/>
+    <mergeCell ref="E77:G77"/>
+    <mergeCell ref="E78:G78"/>
+    <mergeCell ref="E61:G61"/>
+    <mergeCell ref="E62:G62"/>
+    <mergeCell ref="E63:G63"/>
+    <mergeCell ref="E64:G64"/>
+    <mergeCell ref="E65:G65"/>
+    <mergeCell ref="E66:G66"/>
+    <mergeCell ref="E79:G79"/>
+    <mergeCell ref="E80:G80"/>
+    <mergeCell ref="E69:G69"/>
+    <mergeCell ref="E70:G70"/>
+    <mergeCell ref="E71:G71"/>
+    <mergeCell ref="E72:G72"/>
+    <mergeCell ref="E67:G67"/>
+    <mergeCell ref="E68:G68"/>
+    <mergeCell ref="J6:U6"/>
+    <mergeCell ref="J8:U8"/>
+    <mergeCell ref="J9:U9"/>
+    <mergeCell ref="J10:U10"/>
+    <mergeCell ref="J11:U11"/>
+    <mergeCell ref="J12:U12"/>
+    <mergeCell ref="J13:U13"/>
+    <mergeCell ref="J14:U14"/>
+    <mergeCell ref="J15:U15"/>
+    <mergeCell ref="J7:U7"/>
     <mergeCell ref="J16:U16"/>
     <mergeCell ref="J17:U17"/>
     <mergeCell ref="J18:U18"/>
@@ -2886,119 +2993,21 @@
     <mergeCell ref="J34:U34"/>
     <mergeCell ref="J29:U29"/>
     <mergeCell ref="J30:U30"/>
-    <mergeCell ref="J6:U6"/>
-    <mergeCell ref="J8:U8"/>
-    <mergeCell ref="J9:U9"/>
-    <mergeCell ref="J10:U10"/>
-    <mergeCell ref="J11:U11"/>
-    <mergeCell ref="J12:U12"/>
-    <mergeCell ref="J13:U13"/>
-    <mergeCell ref="J14:U14"/>
-    <mergeCell ref="J15:U15"/>
-    <mergeCell ref="J7:U7"/>
-    <mergeCell ref="E81:G81"/>
-    <mergeCell ref="E73:G73"/>
-    <mergeCell ref="E74:G74"/>
-    <mergeCell ref="E75:G75"/>
-    <mergeCell ref="E76:G76"/>
-    <mergeCell ref="E77:G77"/>
-    <mergeCell ref="E78:G78"/>
-    <mergeCell ref="E61:G61"/>
-    <mergeCell ref="E62:G62"/>
-    <mergeCell ref="E63:G63"/>
-    <mergeCell ref="E64:G64"/>
-    <mergeCell ref="E65:G65"/>
-    <mergeCell ref="E66:G66"/>
-    <mergeCell ref="E79:G79"/>
-    <mergeCell ref="E80:G80"/>
-    <mergeCell ref="E69:G69"/>
-    <mergeCell ref="E70:G70"/>
-    <mergeCell ref="E71:G71"/>
-    <mergeCell ref="E72:G72"/>
-    <mergeCell ref="E67:G67"/>
-    <mergeCell ref="E68:G68"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="J77:U77"/>
-    <mergeCell ref="J78:U78"/>
-    <mergeCell ref="J67:U67"/>
-    <mergeCell ref="J68:U68"/>
-    <mergeCell ref="J69:U69"/>
-    <mergeCell ref="J70:U70"/>
-    <mergeCell ref="J65:U65"/>
-    <mergeCell ref="J66:U66"/>
-    <mergeCell ref="J55:U55"/>
-    <mergeCell ref="J56:U56"/>
-    <mergeCell ref="J57:U57"/>
-    <mergeCell ref="J58:U58"/>
-    <mergeCell ref="J53:U53"/>
-    <mergeCell ref="J54:U54"/>
-    <mergeCell ref="J43:U43"/>
-    <mergeCell ref="J44:U44"/>
-    <mergeCell ref="J45:U45"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="J19:U19"/>
-    <mergeCell ref="J20:U20"/>
-    <mergeCell ref="J21:U21"/>
-    <mergeCell ref="J22:U22"/>
-    <mergeCell ref="J23:U23"/>
-    <mergeCell ref="J24:U24"/>
-    <mergeCell ref="J25:U25"/>
-    <mergeCell ref="J26:U26"/>
-    <mergeCell ref="J27:U27"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="J28:U28"/>
-    <mergeCell ref="E57:G57"/>
-    <mergeCell ref="E58:G58"/>
-    <mergeCell ref="E59:G59"/>
-    <mergeCell ref="E60:G60"/>
-    <mergeCell ref="E55:G55"/>
-    <mergeCell ref="E56:G56"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="E51:G51"/>
-    <mergeCell ref="E52:G52"/>
-    <mergeCell ref="E53:G53"/>
-    <mergeCell ref="E54:G54"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="J81:U81"/>
+    <mergeCell ref="J71:U71"/>
+    <mergeCell ref="J72:U72"/>
+    <mergeCell ref="J73:U73"/>
+    <mergeCell ref="J74:U74"/>
+    <mergeCell ref="J75:U75"/>
+    <mergeCell ref="J76:U76"/>
+    <mergeCell ref="J59:U59"/>
+    <mergeCell ref="J60:U60"/>
+    <mergeCell ref="J61:U61"/>
+    <mergeCell ref="J62:U62"/>
+    <mergeCell ref="J63:U63"/>
+    <mergeCell ref="J64:U64"/>
+    <mergeCell ref="J79:U79"/>
+    <mergeCell ref="J80:U80"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3010,8 +3019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF5A0909-FF36-4310-BA25-6FCBC91BB495}">
   <dimension ref="F2:Z74"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9:H9"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10:Y10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3022,11 +3031,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="6:26" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
       <c r="I2" s="8" t="s">
         <v>95</v>
       </c>
@@ -3076,22 +3085,22 @@
         <v>109</v>
       </c>
       <c r="G4" s="8"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="11"/>
-      <c r="S4" s="9"/>
-      <c r="T4" s="10"/>
-      <c r="U4" s="10"/>
-      <c r="V4" s="10"/>
-      <c r="W4" s="11"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
+      <c r="P4" s="14"/>
+      <c r="Q4" s="14"/>
+      <c r="R4" s="15"/>
+      <c r="S4" s="13"/>
+      <c r="T4" s="14"/>
+      <c r="U4" s="14"/>
+      <c r="V4" s="14"/>
+      <c r="W4" s="15"/>
     </row>
     <row r="6" spans="6:26" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F6" s="12" t="s">
@@ -3113,11 +3122,11 @@
       </c>
     </row>
     <row r="7" spans="6:26" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
       <c r="I7" s="1"/>
       <c r="J7" s="6" t="s">
         <v>86</v>
@@ -3206,11 +3215,11 @@
       </c>
     </row>
     <row r="10" spans="6:26" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F10" s="8" t="s">
+      <c r="F10" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1" t="s">
         <v>97</v>
@@ -3237,11 +3246,11 @@
       </c>
     </row>
     <row r="11" spans="6:26" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F11" s="8" t="s">
+      <c r="F11" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1" t="s">
         <v>97</v>
@@ -3330,29 +3339,29 @@
       </c>
     </row>
     <row r="14" spans="6:26" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F14" s="15" t="s">
+      <c r="F14" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="15"/>
-      <c r="M14" s="15"/>
-      <c r="N14" s="15"/>
-      <c r="O14" s="15"/>
-      <c r="P14" s="15"/>
-      <c r="Q14" s="15"/>
-      <c r="R14" s="15"/>
-      <c r="S14" s="15"/>
-      <c r="T14" s="15"/>
-      <c r="U14" s="15"/>
-      <c r="V14" s="15"/>
-      <c r="W14" s="15"/>
-      <c r="X14" s="15"/>
-      <c r="Y14" s="15"/>
-      <c r="Z14" s="15"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="11"/>
+      <c r="P14" s="11"/>
+      <c r="Q14" s="11"/>
+      <c r="R14" s="11"/>
+      <c r="S14" s="11"/>
+      <c r="T14" s="11"/>
+      <c r="U14" s="11"/>
+      <c r="V14" s="11"/>
+      <c r="W14" s="11"/>
+      <c r="X14" s="11"/>
+      <c r="Y14" s="11"/>
+      <c r="Z14" s="11"/>
     </row>
     <row r="15" spans="6:26" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I15" s="1"/>
@@ -4589,6 +4598,120 @@
     </row>
   </sheetData>
   <mergeCells count="138">
+    <mergeCell ref="F73:H73"/>
+    <mergeCell ref="F74:H74"/>
+    <mergeCell ref="F65:H65"/>
+    <mergeCell ref="F66:H66"/>
+    <mergeCell ref="F67:H67"/>
+    <mergeCell ref="F68:H68"/>
+    <mergeCell ref="F69:H69"/>
+    <mergeCell ref="F70:H70"/>
+    <mergeCell ref="S4:W4"/>
+    <mergeCell ref="M4:R4"/>
+    <mergeCell ref="I4:L4"/>
+    <mergeCell ref="L8:Y8"/>
+    <mergeCell ref="F58:H58"/>
+    <mergeCell ref="F59:H59"/>
+    <mergeCell ref="F60:H60"/>
+    <mergeCell ref="F61:H61"/>
+    <mergeCell ref="F62:H62"/>
+    <mergeCell ref="F63:H63"/>
+    <mergeCell ref="F64:H64"/>
+    <mergeCell ref="F71:H71"/>
+    <mergeCell ref="F72:H72"/>
+    <mergeCell ref="F49:H49"/>
+    <mergeCell ref="F50:H50"/>
+    <mergeCell ref="F51:H51"/>
+    <mergeCell ref="F52:H52"/>
+    <mergeCell ref="F53:H53"/>
+    <mergeCell ref="F54:H54"/>
+    <mergeCell ref="F55:H55"/>
+    <mergeCell ref="F56:H56"/>
+    <mergeCell ref="F57:H57"/>
+    <mergeCell ref="F40:H40"/>
+    <mergeCell ref="F41:H41"/>
+    <mergeCell ref="F42:H42"/>
+    <mergeCell ref="F43:H43"/>
+    <mergeCell ref="F44:H44"/>
+    <mergeCell ref="F45:H45"/>
+    <mergeCell ref="F46:H46"/>
+    <mergeCell ref="F47:H47"/>
+    <mergeCell ref="F48:H48"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="F36:H36"/>
+    <mergeCell ref="F37:H37"/>
+    <mergeCell ref="F38:H38"/>
+    <mergeCell ref="F39:H39"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="L16:Y16"/>
+    <mergeCell ref="L17:Y17"/>
+    <mergeCell ref="L18:Y18"/>
+    <mergeCell ref="L19:Y19"/>
+    <mergeCell ref="L20:Y20"/>
+    <mergeCell ref="L21:Y21"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="L7:Y7"/>
+    <mergeCell ref="L12:Y12"/>
+    <mergeCell ref="L9:Y9"/>
+    <mergeCell ref="L13:Y13"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="L11:Y11"/>
+    <mergeCell ref="L31:Y31"/>
+    <mergeCell ref="L32:Y32"/>
+    <mergeCell ref="L33:Y33"/>
+    <mergeCell ref="L22:Y22"/>
+    <mergeCell ref="L23:Y23"/>
+    <mergeCell ref="L24:Y24"/>
+    <mergeCell ref="L25:Y25"/>
+    <mergeCell ref="L26:Y26"/>
+    <mergeCell ref="L27:Y27"/>
+    <mergeCell ref="L68:Y68"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="I2:Z2"/>
+    <mergeCell ref="F14:Z14"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="L15:Y15"/>
+    <mergeCell ref="L58:Y58"/>
+    <mergeCell ref="L59:Y59"/>
+    <mergeCell ref="L60:Y60"/>
+    <mergeCell ref="L61:Y61"/>
+    <mergeCell ref="L62:Y62"/>
+    <mergeCell ref="L63:Y63"/>
+    <mergeCell ref="L52:Y52"/>
+    <mergeCell ref="L53:Y53"/>
+    <mergeCell ref="L54:Y54"/>
+    <mergeCell ref="L55:Y55"/>
+    <mergeCell ref="L56:Y56"/>
+    <mergeCell ref="L57:Y57"/>
+    <mergeCell ref="L46:Y46"/>
+    <mergeCell ref="L47:Y47"/>
+    <mergeCell ref="L48:Y48"/>
+    <mergeCell ref="L49:Y49"/>
+    <mergeCell ref="L50:Y50"/>
+    <mergeCell ref="L51:Y51"/>
     <mergeCell ref="F4:H4"/>
     <mergeCell ref="I3:L3"/>
     <mergeCell ref="M3:R3"/>
@@ -4613,120 +4736,6 @@
     <mergeCell ref="L28:Y28"/>
     <mergeCell ref="L29:Y29"/>
     <mergeCell ref="L30:Y30"/>
-    <mergeCell ref="L68:Y68"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="I2:Z2"/>
-    <mergeCell ref="F14:Z14"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="L15:Y15"/>
-    <mergeCell ref="L58:Y58"/>
-    <mergeCell ref="L59:Y59"/>
-    <mergeCell ref="L60:Y60"/>
-    <mergeCell ref="L61:Y61"/>
-    <mergeCell ref="L62:Y62"/>
-    <mergeCell ref="L63:Y63"/>
-    <mergeCell ref="L52:Y52"/>
-    <mergeCell ref="L53:Y53"/>
-    <mergeCell ref="L54:Y54"/>
-    <mergeCell ref="L55:Y55"/>
-    <mergeCell ref="L56:Y56"/>
-    <mergeCell ref="L57:Y57"/>
-    <mergeCell ref="L46:Y46"/>
-    <mergeCell ref="L47:Y47"/>
-    <mergeCell ref="L48:Y48"/>
-    <mergeCell ref="L49:Y49"/>
-    <mergeCell ref="L50:Y50"/>
-    <mergeCell ref="L51:Y51"/>
-    <mergeCell ref="L31:Y31"/>
-    <mergeCell ref="L32:Y32"/>
-    <mergeCell ref="L33:Y33"/>
-    <mergeCell ref="L22:Y22"/>
-    <mergeCell ref="L23:Y23"/>
-    <mergeCell ref="L24:Y24"/>
-    <mergeCell ref="L25:Y25"/>
-    <mergeCell ref="L26:Y26"/>
-    <mergeCell ref="L27:Y27"/>
-    <mergeCell ref="L16:Y16"/>
-    <mergeCell ref="L17:Y17"/>
-    <mergeCell ref="L18:Y18"/>
-    <mergeCell ref="L19:Y19"/>
-    <mergeCell ref="L20:Y20"/>
-    <mergeCell ref="L21:Y21"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="L7:Y7"/>
-    <mergeCell ref="L12:Y12"/>
-    <mergeCell ref="L9:Y9"/>
-    <mergeCell ref="L13:Y13"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="L11:Y11"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="F25:H25"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="F36:H36"/>
-    <mergeCell ref="F37:H37"/>
-    <mergeCell ref="F38:H38"/>
-    <mergeCell ref="F39:H39"/>
-    <mergeCell ref="F52:H52"/>
-    <mergeCell ref="F53:H53"/>
-    <mergeCell ref="F54:H54"/>
-    <mergeCell ref="F55:H55"/>
-    <mergeCell ref="F56:H56"/>
-    <mergeCell ref="F57:H57"/>
-    <mergeCell ref="F40:H40"/>
-    <mergeCell ref="F41:H41"/>
-    <mergeCell ref="F42:H42"/>
-    <mergeCell ref="F43:H43"/>
-    <mergeCell ref="F44:H44"/>
-    <mergeCell ref="F45:H45"/>
-    <mergeCell ref="F46:H46"/>
-    <mergeCell ref="F47:H47"/>
-    <mergeCell ref="F48:H48"/>
-    <mergeCell ref="F73:H73"/>
-    <mergeCell ref="F74:H74"/>
-    <mergeCell ref="F65:H65"/>
-    <mergeCell ref="F66:H66"/>
-    <mergeCell ref="F67:H67"/>
-    <mergeCell ref="F68:H68"/>
-    <mergeCell ref="F69:H69"/>
-    <mergeCell ref="F70:H70"/>
-    <mergeCell ref="S4:W4"/>
-    <mergeCell ref="M4:R4"/>
-    <mergeCell ref="I4:L4"/>
-    <mergeCell ref="L8:Y8"/>
-    <mergeCell ref="F58:H58"/>
-    <mergeCell ref="F59:H59"/>
-    <mergeCell ref="F60:H60"/>
-    <mergeCell ref="F61:H61"/>
-    <mergeCell ref="F62:H62"/>
-    <mergeCell ref="F63:H63"/>
-    <mergeCell ref="F64:H64"/>
-    <mergeCell ref="F71:H71"/>
-    <mergeCell ref="F72:H72"/>
-    <mergeCell ref="F49:H49"/>
-    <mergeCell ref="F50:H50"/>
-    <mergeCell ref="F51:H51"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update duxing and flash animation
</commit_message>
<xml_diff>
--- a/cards.xlsx
+++ b/cards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\_projects\_OFF\theParasitized\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B72C8B1-9F1D-4C7E-9174-BFAFE45A7BA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30ED4C17-705E-4C29-ADB4-27FF7D1252A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6492" yWindow="816" windowWidth="14616" windowHeight="11340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -672,13 +672,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -687,16 +690,13 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2856,21 +2856,119 @@
     </row>
   </sheetData>
   <mergeCells count="152">
-    <mergeCell ref="J81:U81"/>
-    <mergeCell ref="J71:U71"/>
-    <mergeCell ref="J72:U72"/>
-    <mergeCell ref="J73:U73"/>
-    <mergeCell ref="J74:U74"/>
-    <mergeCell ref="J75:U75"/>
-    <mergeCell ref="J76:U76"/>
-    <mergeCell ref="J59:U59"/>
-    <mergeCell ref="J60:U60"/>
-    <mergeCell ref="J61:U61"/>
-    <mergeCell ref="J62:U62"/>
-    <mergeCell ref="J63:U63"/>
-    <mergeCell ref="J64:U64"/>
-    <mergeCell ref="J79:U79"/>
-    <mergeCell ref="J80:U80"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="J28:U28"/>
+    <mergeCell ref="E57:G57"/>
+    <mergeCell ref="E58:G58"/>
+    <mergeCell ref="E59:G59"/>
+    <mergeCell ref="E60:G60"/>
+    <mergeCell ref="E55:G55"/>
+    <mergeCell ref="E56:G56"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="E51:G51"/>
+    <mergeCell ref="E52:G52"/>
+    <mergeCell ref="E53:G53"/>
+    <mergeCell ref="E54:G54"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="J19:U19"/>
+    <mergeCell ref="J20:U20"/>
+    <mergeCell ref="J21:U21"/>
+    <mergeCell ref="J22:U22"/>
+    <mergeCell ref="J23:U23"/>
+    <mergeCell ref="J24:U24"/>
+    <mergeCell ref="J25:U25"/>
+    <mergeCell ref="J26:U26"/>
+    <mergeCell ref="J27:U27"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="J77:U77"/>
+    <mergeCell ref="J78:U78"/>
+    <mergeCell ref="J67:U67"/>
+    <mergeCell ref="J68:U68"/>
+    <mergeCell ref="J69:U69"/>
+    <mergeCell ref="J70:U70"/>
+    <mergeCell ref="J65:U65"/>
+    <mergeCell ref="J66:U66"/>
+    <mergeCell ref="J55:U55"/>
+    <mergeCell ref="J56:U56"/>
+    <mergeCell ref="J57:U57"/>
+    <mergeCell ref="J58:U58"/>
+    <mergeCell ref="J53:U53"/>
+    <mergeCell ref="J54:U54"/>
+    <mergeCell ref="J43:U43"/>
+    <mergeCell ref="J44:U44"/>
+    <mergeCell ref="J45:U45"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="E81:G81"/>
+    <mergeCell ref="E73:G73"/>
+    <mergeCell ref="E74:G74"/>
+    <mergeCell ref="E75:G75"/>
+    <mergeCell ref="E76:G76"/>
+    <mergeCell ref="E77:G77"/>
+    <mergeCell ref="E78:G78"/>
+    <mergeCell ref="E61:G61"/>
+    <mergeCell ref="E62:G62"/>
+    <mergeCell ref="E63:G63"/>
+    <mergeCell ref="E64:G64"/>
+    <mergeCell ref="E65:G65"/>
+    <mergeCell ref="E66:G66"/>
+    <mergeCell ref="E79:G79"/>
+    <mergeCell ref="E80:G80"/>
+    <mergeCell ref="E69:G69"/>
+    <mergeCell ref="E70:G70"/>
+    <mergeCell ref="E71:G71"/>
+    <mergeCell ref="E72:G72"/>
+    <mergeCell ref="E67:G67"/>
+    <mergeCell ref="E68:G68"/>
+    <mergeCell ref="J6:U6"/>
+    <mergeCell ref="J8:U8"/>
+    <mergeCell ref="J9:U9"/>
+    <mergeCell ref="J10:U10"/>
+    <mergeCell ref="J11:U11"/>
+    <mergeCell ref="J12:U12"/>
+    <mergeCell ref="J13:U13"/>
+    <mergeCell ref="J14:U14"/>
+    <mergeCell ref="J15:U15"/>
+    <mergeCell ref="J7:U7"/>
     <mergeCell ref="J16:U16"/>
     <mergeCell ref="J17:U17"/>
     <mergeCell ref="J18:U18"/>
@@ -2895,119 +2993,21 @@
     <mergeCell ref="J34:U34"/>
     <mergeCell ref="J29:U29"/>
     <mergeCell ref="J30:U30"/>
-    <mergeCell ref="J6:U6"/>
-    <mergeCell ref="J8:U8"/>
-    <mergeCell ref="J9:U9"/>
-    <mergeCell ref="J10:U10"/>
-    <mergeCell ref="J11:U11"/>
-    <mergeCell ref="J12:U12"/>
-    <mergeCell ref="J13:U13"/>
-    <mergeCell ref="J14:U14"/>
-    <mergeCell ref="J15:U15"/>
-    <mergeCell ref="J7:U7"/>
-    <mergeCell ref="E81:G81"/>
-    <mergeCell ref="E73:G73"/>
-    <mergeCell ref="E74:G74"/>
-    <mergeCell ref="E75:G75"/>
-    <mergeCell ref="E76:G76"/>
-    <mergeCell ref="E77:G77"/>
-    <mergeCell ref="E78:G78"/>
-    <mergeCell ref="E61:G61"/>
-    <mergeCell ref="E62:G62"/>
-    <mergeCell ref="E63:G63"/>
-    <mergeCell ref="E64:G64"/>
-    <mergeCell ref="E65:G65"/>
-    <mergeCell ref="E66:G66"/>
-    <mergeCell ref="E79:G79"/>
-    <mergeCell ref="E80:G80"/>
-    <mergeCell ref="E69:G69"/>
-    <mergeCell ref="E70:G70"/>
-    <mergeCell ref="E71:G71"/>
-    <mergeCell ref="E72:G72"/>
-    <mergeCell ref="E67:G67"/>
-    <mergeCell ref="E68:G68"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="J77:U77"/>
-    <mergeCell ref="J78:U78"/>
-    <mergeCell ref="J67:U67"/>
-    <mergeCell ref="J68:U68"/>
-    <mergeCell ref="J69:U69"/>
-    <mergeCell ref="J70:U70"/>
-    <mergeCell ref="J65:U65"/>
-    <mergeCell ref="J66:U66"/>
-    <mergeCell ref="J55:U55"/>
-    <mergeCell ref="J56:U56"/>
-    <mergeCell ref="J57:U57"/>
-    <mergeCell ref="J58:U58"/>
-    <mergeCell ref="J53:U53"/>
-    <mergeCell ref="J54:U54"/>
-    <mergeCell ref="J43:U43"/>
-    <mergeCell ref="J44:U44"/>
-    <mergeCell ref="J45:U45"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="J19:U19"/>
-    <mergeCell ref="J20:U20"/>
-    <mergeCell ref="J21:U21"/>
-    <mergeCell ref="J22:U22"/>
-    <mergeCell ref="J23:U23"/>
-    <mergeCell ref="J24:U24"/>
-    <mergeCell ref="J25:U25"/>
-    <mergeCell ref="J26:U26"/>
-    <mergeCell ref="J27:U27"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="J28:U28"/>
-    <mergeCell ref="E57:G57"/>
-    <mergeCell ref="E58:G58"/>
-    <mergeCell ref="E59:G59"/>
-    <mergeCell ref="E60:G60"/>
-    <mergeCell ref="E55:G55"/>
-    <mergeCell ref="E56:G56"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="E51:G51"/>
-    <mergeCell ref="E52:G52"/>
-    <mergeCell ref="E53:G53"/>
-    <mergeCell ref="E54:G54"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="J81:U81"/>
+    <mergeCell ref="J71:U71"/>
+    <mergeCell ref="J72:U72"/>
+    <mergeCell ref="J73:U73"/>
+    <mergeCell ref="J74:U74"/>
+    <mergeCell ref="J75:U75"/>
+    <mergeCell ref="J76:U76"/>
+    <mergeCell ref="J59:U59"/>
+    <mergeCell ref="J60:U60"/>
+    <mergeCell ref="J61:U61"/>
+    <mergeCell ref="J62:U62"/>
+    <mergeCell ref="J63:U63"/>
+    <mergeCell ref="J64:U64"/>
+    <mergeCell ref="J79:U79"/>
+    <mergeCell ref="J80:U80"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3019,8 +3019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF5A0909-FF36-4310-BA25-6FCBC91BB495}">
   <dimension ref="F2:Z74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3031,11 +3031,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="6:26" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
       <c r="I2" s="8" t="s">
         <v>95</v>
       </c>
@@ -3085,29 +3085,29 @@
         <v>109</v>
       </c>
       <c r="G4" s="8"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="11"/>
-      <c r="S4" s="9"/>
-      <c r="T4" s="10"/>
-      <c r="U4" s="10"/>
-      <c r="V4" s="10"/>
-      <c r="W4" s="11"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="16"/>
+      <c r="P4" s="16"/>
+      <c r="Q4" s="16"/>
+      <c r="R4" s="17"/>
+      <c r="S4" s="15"/>
+      <c r="T4" s="16"/>
+      <c r="U4" s="16"/>
+      <c r="V4" s="16"/>
+      <c r="W4" s="17"/>
     </row>
     <row r="6" spans="6:26" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
       <c r="I6" t="s">
         <v>85</v>
       </c>
@@ -3122,11 +3122,11 @@
       </c>
     </row>
     <row r="7" spans="6:26" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
       <c r="I7" s="1"/>
       <c r="J7" s="6" t="s">
         <v>86</v>
@@ -3184,11 +3184,11 @@
       </c>
     </row>
     <row r="9" spans="6:26" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1" t="s">
         <v>97</v>
@@ -3215,11 +3215,11 @@
       </c>
     </row>
     <row r="10" spans="6:26" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F10" s="14" t="s">
+      <c r="F10" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1" t="s">
         <v>97</v>
@@ -3246,11 +3246,11 @@
       </c>
     </row>
     <row r="11" spans="6:26" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F11" s="14" t="s">
+      <c r="F11" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1" t="s">
         <v>97</v>
@@ -3308,11 +3308,11 @@
       </c>
     </row>
     <row r="13" spans="6:26" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F13" s="14" t="s">
+      <c r="F13" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1" t="s">
         <v>97</v>
@@ -3339,29 +3339,29 @@
       </c>
     </row>
     <row r="14" spans="6:26" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F14" s="16" t="s">
+      <c r="F14" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="16"/>
-      <c r="K14" s="16"/>
-      <c r="L14" s="16"/>
-      <c r="M14" s="16"/>
-      <c r="N14" s="16"/>
-      <c r="O14" s="16"/>
-      <c r="P14" s="16"/>
-      <c r="Q14" s="16"/>
-      <c r="R14" s="16"/>
-      <c r="S14" s="16"/>
-      <c r="T14" s="16"/>
-      <c r="U14" s="16"/>
-      <c r="V14" s="16"/>
-      <c r="W14" s="16"/>
-      <c r="X14" s="16"/>
-      <c r="Y14" s="16"/>
-      <c r="Z14" s="16"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="11"/>
+      <c r="P14" s="11"/>
+      <c r="Q14" s="11"/>
+      <c r="R14" s="11"/>
+      <c r="S14" s="11"/>
+      <c r="T14" s="11"/>
+      <c r="U14" s="11"/>
+      <c r="V14" s="11"/>
+      <c r="W14" s="11"/>
+      <c r="X14" s="11"/>
+      <c r="Y14" s="11"/>
+      <c r="Z14" s="11"/>
     </row>
     <row r="15" spans="6:26" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I15" s="1"/>
@@ -4598,6 +4598,120 @@
     </row>
   </sheetData>
   <mergeCells count="138">
+    <mergeCell ref="F73:H73"/>
+    <mergeCell ref="F74:H74"/>
+    <mergeCell ref="F65:H65"/>
+    <mergeCell ref="F66:H66"/>
+    <mergeCell ref="F67:H67"/>
+    <mergeCell ref="F68:H68"/>
+    <mergeCell ref="F69:H69"/>
+    <mergeCell ref="F70:H70"/>
+    <mergeCell ref="S4:W4"/>
+    <mergeCell ref="M4:R4"/>
+    <mergeCell ref="I4:L4"/>
+    <mergeCell ref="L8:Y8"/>
+    <mergeCell ref="F58:H58"/>
+    <mergeCell ref="F59:H59"/>
+    <mergeCell ref="F60:H60"/>
+    <mergeCell ref="F61:H61"/>
+    <mergeCell ref="F62:H62"/>
+    <mergeCell ref="F63:H63"/>
+    <mergeCell ref="F64:H64"/>
+    <mergeCell ref="F71:H71"/>
+    <mergeCell ref="F72:H72"/>
+    <mergeCell ref="F49:H49"/>
+    <mergeCell ref="F50:H50"/>
+    <mergeCell ref="F51:H51"/>
+    <mergeCell ref="F52:H52"/>
+    <mergeCell ref="F53:H53"/>
+    <mergeCell ref="F54:H54"/>
+    <mergeCell ref="F55:H55"/>
+    <mergeCell ref="F56:H56"/>
+    <mergeCell ref="F57:H57"/>
+    <mergeCell ref="F40:H40"/>
+    <mergeCell ref="F41:H41"/>
+    <mergeCell ref="F42:H42"/>
+    <mergeCell ref="F43:H43"/>
+    <mergeCell ref="F44:H44"/>
+    <mergeCell ref="F45:H45"/>
+    <mergeCell ref="F46:H46"/>
+    <mergeCell ref="F47:H47"/>
+    <mergeCell ref="F48:H48"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="F36:H36"/>
+    <mergeCell ref="F37:H37"/>
+    <mergeCell ref="F38:H38"/>
+    <mergeCell ref="F39:H39"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="L16:Y16"/>
+    <mergeCell ref="L17:Y17"/>
+    <mergeCell ref="L18:Y18"/>
+    <mergeCell ref="L19:Y19"/>
+    <mergeCell ref="L20:Y20"/>
+    <mergeCell ref="L21:Y21"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="L7:Y7"/>
+    <mergeCell ref="L12:Y12"/>
+    <mergeCell ref="L9:Y9"/>
+    <mergeCell ref="L13:Y13"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="L11:Y11"/>
+    <mergeCell ref="L31:Y31"/>
+    <mergeCell ref="L32:Y32"/>
+    <mergeCell ref="L33:Y33"/>
+    <mergeCell ref="L22:Y22"/>
+    <mergeCell ref="L23:Y23"/>
+    <mergeCell ref="L24:Y24"/>
+    <mergeCell ref="L25:Y25"/>
+    <mergeCell ref="L26:Y26"/>
+    <mergeCell ref="L27:Y27"/>
+    <mergeCell ref="L68:Y68"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="I2:Z2"/>
+    <mergeCell ref="F14:Z14"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="L15:Y15"/>
+    <mergeCell ref="L58:Y58"/>
+    <mergeCell ref="L59:Y59"/>
+    <mergeCell ref="L60:Y60"/>
+    <mergeCell ref="L61:Y61"/>
+    <mergeCell ref="L62:Y62"/>
+    <mergeCell ref="L63:Y63"/>
+    <mergeCell ref="L52:Y52"/>
+    <mergeCell ref="L53:Y53"/>
+    <mergeCell ref="L54:Y54"/>
+    <mergeCell ref="L55:Y55"/>
+    <mergeCell ref="L56:Y56"/>
+    <mergeCell ref="L57:Y57"/>
+    <mergeCell ref="L46:Y46"/>
+    <mergeCell ref="L47:Y47"/>
+    <mergeCell ref="L48:Y48"/>
+    <mergeCell ref="L49:Y49"/>
+    <mergeCell ref="L50:Y50"/>
+    <mergeCell ref="L51:Y51"/>
     <mergeCell ref="F4:H4"/>
     <mergeCell ref="I3:L3"/>
     <mergeCell ref="M3:R3"/>
@@ -4622,120 +4736,6 @@
     <mergeCell ref="L28:Y28"/>
     <mergeCell ref="L29:Y29"/>
     <mergeCell ref="L30:Y30"/>
-    <mergeCell ref="L68:Y68"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="I2:Z2"/>
-    <mergeCell ref="F14:Z14"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="L15:Y15"/>
-    <mergeCell ref="L58:Y58"/>
-    <mergeCell ref="L59:Y59"/>
-    <mergeCell ref="L60:Y60"/>
-    <mergeCell ref="L61:Y61"/>
-    <mergeCell ref="L62:Y62"/>
-    <mergeCell ref="L63:Y63"/>
-    <mergeCell ref="L52:Y52"/>
-    <mergeCell ref="L53:Y53"/>
-    <mergeCell ref="L54:Y54"/>
-    <mergeCell ref="L55:Y55"/>
-    <mergeCell ref="L56:Y56"/>
-    <mergeCell ref="L57:Y57"/>
-    <mergeCell ref="L46:Y46"/>
-    <mergeCell ref="L47:Y47"/>
-    <mergeCell ref="L48:Y48"/>
-    <mergeCell ref="L49:Y49"/>
-    <mergeCell ref="L50:Y50"/>
-    <mergeCell ref="L51:Y51"/>
-    <mergeCell ref="L31:Y31"/>
-    <mergeCell ref="L32:Y32"/>
-    <mergeCell ref="L33:Y33"/>
-    <mergeCell ref="L22:Y22"/>
-    <mergeCell ref="L23:Y23"/>
-    <mergeCell ref="L24:Y24"/>
-    <mergeCell ref="L25:Y25"/>
-    <mergeCell ref="L26:Y26"/>
-    <mergeCell ref="L27:Y27"/>
-    <mergeCell ref="L16:Y16"/>
-    <mergeCell ref="L17:Y17"/>
-    <mergeCell ref="L18:Y18"/>
-    <mergeCell ref="L19:Y19"/>
-    <mergeCell ref="L20:Y20"/>
-    <mergeCell ref="L21:Y21"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="L7:Y7"/>
-    <mergeCell ref="L12:Y12"/>
-    <mergeCell ref="L9:Y9"/>
-    <mergeCell ref="L13:Y13"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="L11:Y11"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="F25:H25"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="F36:H36"/>
-    <mergeCell ref="F37:H37"/>
-    <mergeCell ref="F38:H38"/>
-    <mergeCell ref="F39:H39"/>
-    <mergeCell ref="F52:H52"/>
-    <mergeCell ref="F53:H53"/>
-    <mergeCell ref="F54:H54"/>
-    <mergeCell ref="F55:H55"/>
-    <mergeCell ref="F56:H56"/>
-    <mergeCell ref="F57:H57"/>
-    <mergeCell ref="F40:H40"/>
-    <mergeCell ref="F41:H41"/>
-    <mergeCell ref="F42:H42"/>
-    <mergeCell ref="F43:H43"/>
-    <mergeCell ref="F44:H44"/>
-    <mergeCell ref="F45:H45"/>
-    <mergeCell ref="F46:H46"/>
-    <mergeCell ref="F47:H47"/>
-    <mergeCell ref="F48:H48"/>
-    <mergeCell ref="F73:H73"/>
-    <mergeCell ref="F74:H74"/>
-    <mergeCell ref="F65:H65"/>
-    <mergeCell ref="F66:H66"/>
-    <mergeCell ref="F67:H67"/>
-    <mergeCell ref="F68:H68"/>
-    <mergeCell ref="F69:H69"/>
-    <mergeCell ref="F70:H70"/>
-    <mergeCell ref="S4:W4"/>
-    <mergeCell ref="M4:R4"/>
-    <mergeCell ref="I4:L4"/>
-    <mergeCell ref="L8:Y8"/>
-    <mergeCell ref="F58:H58"/>
-    <mergeCell ref="F59:H59"/>
-    <mergeCell ref="F60:H60"/>
-    <mergeCell ref="F61:H61"/>
-    <mergeCell ref="F62:H62"/>
-    <mergeCell ref="F63:H63"/>
-    <mergeCell ref="F64:H64"/>
-    <mergeCell ref="F71:H71"/>
-    <mergeCell ref="F72:H72"/>
-    <mergeCell ref="F49:H49"/>
-    <mergeCell ref="F50:H50"/>
-    <mergeCell ref="F51:H51"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>